<commit_message>
new system for str
</commit_message>
<xml_diff>
--- a/assets/i9sa.xlsx
+++ b/assets/i9sa.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demet\go\i9esareal\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9-esa/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F935950C-9956-4868-A358-0EA0D519F6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ref" sheetId="2" r:id="rId1"/>
     <sheet name="Main" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Main!$A$1:$F$59</definedName>
+    <definedName hidden="true" localSheetId="1" name="_xlnm._FilterDatabase">Main!$A$1:$F$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="175">
   <si>
     <t>Name</t>
   </si>
@@ -544,13 +543,34 @@
   </si>
   <si>
     <t>Weight Value</t>
+  </si>
+  <si>
+    <t>667cd55c52e83b24dbfe229a</t>
+  </si>
+  <si>
+    <t>667cd55d52e83b24dbfe229b</t>
+  </si>
+  <si>
+    <t>667cd55d52e83b24dbfe229d</t>
+  </si>
+  <si>
+    <t>667cd55d52e83b24dbfe22a0</t>
+  </si>
+  <si>
+    <t>667cd55d52e83b24dbfe229f</t>
+  </si>
+  <si>
+    <t>667cd55d52e83b24dbfe229c</t>
+  </si>
+  <si>
+    <t>667cd55d52e83b24dbfe229e</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,7 +593,7 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -581,7 +601,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -589,7 +609,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -625,7 +645,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -633,7 +653,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -648,7 +668,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -663,7 +683,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <i val="1"/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -671,7 +691,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -735,19 +755,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -758,19 +778,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -781,19 +801,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -804,19 +824,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -827,19 +847,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -850,19 +870,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -898,7 +918,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.3999755851924192"/>
       </bottom>
       <diagonal/>
     </border>
@@ -985,95 +1005,95 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="true"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="true"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="true"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="true"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="true"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="true"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="true"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="true"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="true"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="true"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="true"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="true"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="true"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="true"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="true"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="true"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="true"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="true"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="true"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="true"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="true"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="true"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="true"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="true"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="true"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="true"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="true"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="true"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="true"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="true"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="true"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="true"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="true"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="true"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="true"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1084,7 +1104,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1097,154 +1117,154 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
-      <a:fillStyleLst>
+<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office 2013 - 2022 Theme">
+  <themeElements>
+    <clrScheme name="Office 2013 - 2022">
+      <dk1>
+        <sysClr val="windowText" lastClr="000000"/>
+      </dk1>
+      <lt1>
+        <sysClr val="window" lastClr="FFFFFF"/>
+      </lt1>
+      <dk2>
+        <srgbClr val="44546A"/>
+      </dk2>
+      <lt2>
+        <srgbClr val="E7E6E6"/>
+      </lt2>
+      <accent1>
+        <srgbClr val="4472C4"/>
+      </accent1>
+      <accent2>
+        <srgbClr val="ED7D31"/>
+      </accent2>
+      <accent3>
+        <srgbClr val="A5A5A5"/>
+      </accent3>
+      <accent4>
+        <srgbClr val="FFC000"/>
+      </accent4>
+      <accent5>
+        <srgbClr val="5B9BD5"/>
+      </accent5>
+      <accent6>
+        <srgbClr val="70AD47"/>
+      </accent6>
+      <hlink>
+        <srgbClr val="0563C1"/>
+      </hlink>
+      <folHlink>
+        <srgbClr val="954F72"/>
+      </folHlink>
+    </clrScheme>
+    <fontScheme name="Office 2013 - 2022">
+      <majorFont>
+        <latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="游ゴシック Light"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线 Light"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Times New Roman"/>
+        <font script="Hebr" typeface="Times New Roman"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="MoolBoran"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Times New Roman"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+        <font script="Armn" typeface="Arial"/>
+        <font script="Bugi" typeface="Leelawadee UI"/>
+        <font script="Bopo" typeface="Microsoft JhengHei"/>
+        <font script="Java" typeface="Javanese Text"/>
+        <font script="Lisu" typeface="Segoe UI"/>
+        <font script="Mymr" typeface="Myanmar Text"/>
+        <font script="Nkoo" typeface="Ebrima"/>
+        <font script="Olck" typeface="Nirmala UI"/>
+        <font script="Osma" typeface="Ebrima"/>
+        <font script="Phag" typeface="Phagspa"/>
+        <font script="Syrn" typeface="Estrangelo Edessa"/>
+        <font script="Syrj" typeface="Estrangelo Edessa"/>
+        <font script="Syre" typeface="Estrangelo Edessa"/>
+        <font script="Sora" typeface="Nirmala UI"/>
+        <font script="Tale" typeface="Microsoft Tai Le"/>
+        <font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <font script="Tfng" typeface="Ebrima"/>
+      </majorFont>
+      <minorFont>
+        <latin typeface="Calibri" panose="020F0502020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="游ゴシック"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Arial"/>
+        <font script="Hebr" typeface="Arial"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="DaunPenh"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Arial"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+        <font script="Armn" typeface="Arial"/>
+        <font script="Bugi" typeface="Leelawadee UI"/>
+        <font script="Bopo" typeface="Microsoft JhengHei"/>
+        <font script="Java" typeface="Javanese Text"/>
+        <font script="Lisu" typeface="Segoe UI"/>
+        <font script="Mymr" typeface="Myanmar Text"/>
+        <font script="Nkoo" typeface="Ebrima"/>
+        <font script="Olck" typeface="Nirmala UI"/>
+        <font script="Osma" typeface="Ebrima"/>
+        <font script="Phag" typeface="Phagspa"/>
+        <font script="Syrn" typeface="Estrangelo Edessa"/>
+        <font script="Syrj" typeface="Estrangelo Edessa"/>
+        <font script="Syre" typeface="Estrangelo Edessa"/>
+        <font script="Sora" typeface="Nirmala UI"/>
+        <font script="Tale" typeface="Microsoft Tai Le"/>
+        <font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <font script="Tfng" typeface="Ebrima"/>
+      </minorFont>
+    </fontScheme>
+    <fmtScheme name="Office 2013 - 2022">
+      <fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1300,8 +1320,8 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
+      </fillStyleLst>
+      <lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1323,8 +1343,8 @@
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
+      </lnStyleLst>
+      <effectStyleLst>
         <a:effectStyle>
           <a:effectLst/>
         </a:effectStyle>
@@ -1340,8 +1360,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
+      </effectStyleLst>
+      <bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1378,17 +1398,17 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
+      </bgFillStyleLst>
+    </fmtScheme>
+  </themeElements>
+  <objectDefaults/>
+  <extraClrSchemeLst/>
+  <extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
       <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
-  </a:extLst>
-</a:theme>
+  </extLst>
+</theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1399,13 +1419,13 @@
       <selection activeCell="B2" sqref="A2:B152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col bestFit="true" customWidth="true" max="1" min="1" width="19.6640625"/>
+    <col bestFit="true" customWidth="true" max="2" min="2" width="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -1413,7 +1433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1421,7 +1441,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1429,7 +1449,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1437,7 +1457,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -1445,7 +1465,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1453,7 +1473,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1461,7 +1481,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1469,7 +1489,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1477,7 +1497,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1485,7 +1505,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1493,7 +1513,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1501,7 +1521,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1509,7 +1529,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1517,7 +1537,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -1525,7 +1545,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1533,7 +1553,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1541,7 +1561,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1549,7 +1569,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -1557,7 +1577,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1565,7 +1585,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1573,7 +1593,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1581,7 +1601,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1589,7 +1609,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1597,7 +1617,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1605,7 +1625,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1613,7 +1633,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -1621,7 +1641,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -1629,7 +1649,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1637,7 +1657,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1645,7 +1665,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1653,7 +1673,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1661,7 +1681,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1669,7 +1689,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1677,7 +1697,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1685,7 +1705,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1693,7 +1713,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -1701,7 +1721,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -1709,7 +1729,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -1717,7 +1737,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1725,7 +1745,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1733,7 +1753,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1741,7 +1761,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -1749,7 +1769,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1757,7 +1777,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1765,7 +1785,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -1773,7 +1793,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -1781,7 +1801,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -1789,7 +1809,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -1797,7 +1817,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -1805,7 +1825,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>99</v>
       </c>
@@ -1813,7 +1833,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>81</v>
       </c>
@@ -1821,7 +1841,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>95</v>
       </c>
@@ -1829,7 +1849,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1837,7 +1857,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -1845,7 +1865,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>46</v>
       </c>
@@ -1853,7 +1873,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -1861,7 +1881,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>97</v>
       </c>
@@ -1869,7 +1889,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -1877,7 +1897,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -1885,7 +1905,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -1893,7 +1913,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>96</v>
       </c>
@@ -1901,7 +1921,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>91</v>
       </c>
@@ -1909,7 +1929,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -1917,7 +1937,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>85</v>
       </c>
@@ -1925,7 +1945,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>51</v>
       </c>
@@ -1933,7 +1953,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>44</v>
       </c>
@@ -1941,7 +1961,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -1949,7 +1969,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -1957,7 +1977,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -1965,7 +1985,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>94</v>
       </c>
@@ -1973,7 +1993,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>30</v>
       </c>
@@ -1981,7 +2001,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>31</v>
       </c>
@@ -1989,7 +2009,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>36</v>
       </c>
@@ -1997,7 +2017,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -2005,7 +2025,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>45</v>
       </c>
@@ -2013,7 +2033,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2021,7 +2041,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>37</v>
       </c>
@@ -2029,7 +2049,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>53</v>
       </c>
@@ -2037,7 +2057,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -2045,7 +2065,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>28</v>
       </c>
@@ -2053,7 +2073,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>35</v>
       </c>
@@ -2061,7 +2081,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -2069,7 +2089,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -2077,7 +2097,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>27</v>
       </c>
@@ -2085,7 +2105,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -2093,7 +2113,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>29</v>
       </c>
@@ -2101,7 +2121,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>32</v>
       </c>
@@ -2109,7 +2129,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>33</v>
       </c>
@@ -2117,7 +2137,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>38</v>
       </c>
@@ -2125,7 +2145,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>52</v>
       </c>
@@ -2133,7 +2153,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>41</v>
       </c>
@@ -2141,7 +2161,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -2149,7 +2169,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>34</v>
       </c>
@@ -2157,7 +2177,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
         <v>43</v>
       </c>
@@ -2165,7 +2185,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -2173,7 +2193,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2">
       <c r="A97" t="s">
         <v>81</v>
       </c>
@@ -2181,7 +2201,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98" t="s">
         <v>93</v>
       </c>
@@ -2189,7 +2209,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>26</v>
       </c>
@@ -2197,7 +2217,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -2205,7 +2225,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2">
       <c r="A101" t="s">
         <v>40</v>
       </c>
@@ -2213,7 +2233,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2">
       <c r="A102" t="s">
         <v>50</v>
       </c>
@@ -2221,12 +2241,1868 @@
         <v>144</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2">
       <c r="A103" t="s">
         <v>75</v>
       </c>
       <c r="B103" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>38</v>
+      </c>
+      <c r="B104" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>40</v>
+      </c>
+      <c r="B105" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>46</v>
+      </c>
+      <c r="B106" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>50</v>
+      </c>
+      <c r="B107" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>158</v>
+      </c>
+      <c r="B108" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>156</v>
+      </c>
+      <c r="B109" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>28</v>
+      </c>
+      <c r="B110" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>30</v>
+      </c>
+      <c r="B111" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>88</v>
+      </c>
+      <c r="B112" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>34</v>
+      </c>
+      <c r="B113" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>81</v>
+      </c>
+      <c r="B114" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>33</v>
+      </c>
+      <c r="B115" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>159</v>
+      </c>
+      <c r="B116" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>90</v>
+      </c>
+      <c r="B117" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>51</v>
+      </c>
+      <c r="B118" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>89</v>
+      </c>
+      <c r="B119" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>75</v>
+      </c>
+      <c r="B120" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>87</v>
+      </c>
+      <c r="B121" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>93</v>
+      </c>
+      <c r="B122" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>157</v>
+      </c>
+      <c r="B123" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>44</v>
+      </c>
+      <c r="B124" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>48</v>
+      </c>
+      <c r="B125" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>32</v>
+      </c>
+      <c r="B126" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>79</v>
+      </c>
+      <c r="B127" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>83</v>
+      </c>
+      <c r="B128" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>36</v>
+      </c>
+      <c r="B129" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>37</v>
+      </c>
+      <c r="B130" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>95</v>
+      </c>
+      <c r="B131" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>27</v>
+      </c>
+      <c r="B132" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>47</v>
+      </c>
+      <c r="B133" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>99</v>
+      </c>
+      <c r="B134" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>82</v>
+      </c>
+      <c r="B135" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>94</v>
+      </c>
+      <c r="B136" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>85</v>
+      </c>
+      <c r="B137" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>96</v>
+      </c>
+      <c r="B138" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>26</v>
+      </c>
+      <c r="B139" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>42</v>
+      </c>
+      <c r="B140" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>53</v>
+      </c>
+      <c r="B141" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>70</v>
+      </c>
+      <c r="B142" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>154</v>
+      </c>
+      <c r="B143" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>29</v>
+      </c>
+      <c r="B144" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>49</v>
+      </c>
+      <c r="B145" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>80</v>
+      </c>
+      <c r="B146" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>91</v>
+      </c>
+      <c r="B147" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>155</v>
+      </c>
+      <c r="B148" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>35</v>
+      </c>
+      <c r="B149" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>43</v>
+      </c>
+      <c r="B150" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>66</v>
+      </c>
+      <c r="B151" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>77</v>
+      </c>
+      <c r="B152" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>31</v>
+      </c>
+      <c r="B153" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>52</v>
+      </c>
+      <c r="B154" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>152</v>
+      </c>
+      <c r="B155" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>39</v>
+      </c>
+      <c r="B156" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>69</v>
+      </c>
+      <c r="B157" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>45</v>
+      </c>
+      <c r="B158" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>97</v>
+      </c>
+      <c r="B159" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>41</v>
+      </c>
+      <c r="B160" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>71</v>
+      </c>
+      <c r="B161" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>89</v>
+      </c>
+      <c r="B162" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>91</v>
+      </c>
+      <c r="B163" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>97</v>
+      </c>
+      <c r="B164" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>159</v>
+      </c>
+      <c r="B165" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>32</v>
+      </c>
+      <c r="B166" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>31</v>
+      </c>
+      <c r="B167" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>44</v>
+      </c>
+      <c r="B168" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>85</v>
+      </c>
+      <c r="B169" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>51</v>
+      </c>
+      <c r="B170" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>46</v>
+      </c>
+      <c r="B171" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>83</v>
+      </c>
+      <c r="B172" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>152</v>
+      </c>
+      <c r="B173" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>45</v>
+      </c>
+      <c r="B174" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>47</v>
+      </c>
+      <c r="B175" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>81</v>
+      </c>
+      <c r="B176" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>79</v>
+      </c>
+      <c r="B177" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>87</v>
+      </c>
+      <c r="B178" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>96</v>
+      </c>
+      <c r="B179" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>38</v>
+      </c>
+      <c r="B180" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>71</v>
+      </c>
+      <c r="B181" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>48</v>
+      </c>
+      <c r="B182" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>154</v>
+      </c>
+      <c r="B183" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>27</v>
+      </c>
+      <c r="B184" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>43</v>
+      </c>
+      <c r="B185" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>88</v>
+      </c>
+      <c r="B186" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>99</v>
+      </c>
+      <c r="B187" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>30</v>
+      </c>
+      <c r="B188" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>70</v>
+      </c>
+      <c r="B189" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>80</v>
+      </c>
+      <c r="B190" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>29</v>
+      </c>
+      <c r="B191" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>77</v>
+      </c>
+      <c r="B192" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>53</v>
+      </c>
+      <c r="B193" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>156</v>
+      </c>
+      <c r="B194" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>66</v>
+      </c>
+      <c r="B195" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>90</v>
+      </c>
+      <c r="B196" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>33</v>
+      </c>
+      <c r="B197" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>40</v>
+      </c>
+      <c r="B198" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>49</v>
+      </c>
+      <c r="B199" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>157</v>
+      </c>
+      <c r="B200" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>34</v>
+      </c>
+      <c r="B201" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>36</v>
+      </c>
+      <c r="B202" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>94</v>
+      </c>
+      <c r="B203" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>50</v>
+      </c>
+      <c r="B204" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>75</v>
+      </c>
+      <c r="B205" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>82</v>
+      </c>
+      <c r="B206" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>158</v>
+      </c>
+      <c r="B207" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>35</v>
+      </c>
+      <c r="B208" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>69</v>
+      </c>
+      <c r="B209" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>95</v>
+      </c>
+      <c r="B210" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>26</v>
+      </c>
+      <c r="B211" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>39</v>
+      </c>
+      <c r="B212" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>155</v>
+      </c>
+      <c r="B213" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>42</v>
+      </c>
+      <c r="B214" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>52</v>
+      </c>
+      <c r="B215" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>93</v>
+      </c>
+      <c r="B216" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s">
+        <v>28</v>
+      </c>
+      <c r="B217" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s">
+        <v>37</v>
+      </c>
+      <c r="B218" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s">
+        <v>41</v>
+      </c>
+      <c r="B219" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s">
+        <v>91</v>
+      </c>
+      <c r="B220" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s">
+        <v>88</v>
+      </c>
+      <c r="B221" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s">
+        <v>36</v>
+      </c>
+      <c r="B222" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s">
+        <v>45</v>
+      </c>
+      <c r="B223" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s">
+        <v>47</v>
+      </c>
+      <c r="B224" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s">
+        <v>83</v>
+      </c>
+      <c r="B225" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>34</v>
+      </c>
+      <c r="B226" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>51</v>
+      </c>
+      <c r="B227" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>28</v>
+      </c>
+      <c r="B228" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>31</v>
+      </c>
+      <c r="B229" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>35</v>
+      </c>
+      <c r="B230" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>49</v>
+      </c>
+      <c r="B231" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>75</v>
+      </c>
+      <c r="B232" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>96</v>
+      </c>
+      <c r="B233" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>158</v>
+      </c>
+      <c r="B234" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>32</v>
+      </c>
+      <c r="B235" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>157</v>
+      </c>
+      <c r="B236" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>154</v>
+      </c>
+      <c r="B237" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>50</v>
+      </c>
+      <c r="B238" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>66</v>
+      </c>
+      <c r="B239" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>94</v>
+      </c>
+      <c r="B240" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>155</v>
+      </c>
+      <c r="B241" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>159</v>
+      </c>
+      <c r="B242" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>38</v>
+      </c>
+      <c r="B243" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>43</v>
+      </c>
+      <c r="B244" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>48</v>
+      </c>
+      <c r="B245" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>77</v>
+      </c>
+      <c r="B246" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>97</v>
+      </c>
+      <c r="B247" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>26</v>
+      </c>
+      <c r="B248" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>44</v>
+      </c>
+      <c r="B249" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s">
+        <v>33</v>
+      </c>
+      <c r="B250" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>40</v>
+      </c>
+      <c r="B251" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>71</v>
+      </c>
+      <c r="B252" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>80</v>
+      </c>
+      <c r="B253" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>152</v>
+      </c>
+      <c r="B254" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>37</v>
+      </c>
+      <c r="B255" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>90</v>
+      </c>
+      <c r="B256" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>79</v>
+      </c>
+      <c r="B257" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>85</v>
+      </c>
+      <c r="B258" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>87</v>
+      </c>
+      <c r="B259" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>93</v>
+      </c>
+      <c r="B260" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>41</v>
+      </c>
+      <c r="B261" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s">
+        <v>82</v>
+      </c>
+      <c r="B262" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s">
+        <v>81</v>
+      </c>
+      <c r="B263" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s">
+        <v>46</v>
+      </c>
+      <c r="B264" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>52</v>
+      </c>
+      <c r="B265" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>42</v>
+      </c>
+      <c r="B266" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>53</v>
+      </c>
+      <c r="B267" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
+        <v>70</v>
+      </c>
+      <c r="B268" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s">
+        <v>95</v>
+      </c>
+      <c r="B269" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s">
+        <v>156</v>
+      </c>
+      <c r="B270" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s">
+        <v>39</v>
+      </c>
+      <c r="B271" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s">
+        <v>30</v>
+      </c>
+      <c r="B272" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s">
+        <v>69</v>
+      </c>
+      <c r="B273" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s">
+        <v>27</v>
+      </c>
+      <c r="B274" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s">
+        <v>29</v>
+      </c>
+      <c r="B275" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s">
+        <v>99</v>
+      </c>
+      <c r="B276" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s">
+        <v>89</v>
+      </c>
+      <c r="B277" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s">
+        <v>152</v>
+      </c>
+      <c r="B278" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s">
+        <v>51</v>
+      </c>
+      <c r="B279" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s">
+        <v>41</v>
+      </c>
+      <c r="B280" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>46</v>
+      </c>
+      <c r="B281" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s">
+        <v>49</v>
+      </c>
+      <c r="B282" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s">
+        <v>70</v>
+      </c>
+      <c r="B283" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>81</v>
+      </c>
+      <c r="B284" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>37</v>
+      </c>
+      <c r="B285" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>39</v>
+      </c>
+      <c r="B286" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>44</v>
+      </c>
+      <c r="B287" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>158</v>
+      </c>
+      <c r="B288" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>83</v>
+      </c>
+      <c r="B289" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>91</v>
+      </c>
+      <c r="B290" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>96</v>
+      </c>
+      <c r="B291" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>97</v>
+      </c>
+      <c r="B292" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>82</v>
+      </c>
+      <c r="B293" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>89</v>
+      </c>
+      <c r="B294" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>155</v>
+      </c>
+      <c r="B295" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>154</v>
+      </c>
+      <c r="B296" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>28</v>
+      </c>
+      <c r="B297" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>75</v>
+      </c>
+      <c r="B298" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>79</v>
+      </c>
+      <c r="B299" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>87</v>
+      </c>
+      <c r="B300" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>29</v>
+      </c>
+      <c r="B301" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>50</v>
+      </c>
+      <c r="B302" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s">
+        <v>66</v>
+      </c>
+      <c r="B303" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s">
+        <v>88</v>
+      </c>
+      <c r="B304" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s">
+        <v>52</v>
+      </c>
+      <c r="B305" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s">
+        <v>53</v>
+      </c>
+      <c r="B306" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="s">
+        <v>156</v>
+      </c>
+      <c r="B307" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="s">
+        <v>157</v>
+      </c>
+      <c r="B308" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="s">
+        <v>95</v>
+      </c>
+      <c r="B309" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="s">
+        <v>99</v>
+      </c>
+      <c r="B310" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="s">
+        <v>35</v>
+      </c>
+      <c r="B311" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="s">
+        <v>36</v>
+      </c>
+      <c r="B312" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s">
+        <v>43</v>
+      </c>
+      <c r="B313" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="s">
+        <v>94</v>
+      </c>
+      <c r="B314" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s">
+        <v>31</v>
+      </c>
+      <c r="B315" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s">
+        <v>34</v>
+      </c>
+      <c r="B316" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s">
+        <v>42</v>
+      </c>
+      <c r="B317" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s">
+        <v>32</v>
+      </c>
+      <c r="B318" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s">
+        <v>33</v>
+      </c>
+      <c r="B319" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s">
+        <v>90</v>
+      </c>
+      <c r="B320" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s">
+        <v>93</v>
+      </c>
+      <c r="B321" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s">
+        <v>38</v>
+      </c>
+      <c r="B322" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s">
+        <v>45</v>
+      </c>
+      <c r="B323" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s">
+        <v>48</v>
+      </c>
+      <c r="B324" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s">
+        <v>77</v>
+      </c>
+      <c r="B325" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s">
+        <v>80</v>
+      </c>
+      <c r="B326" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s">
+        <v>27</v>
+      </c>
+      <c r="B327" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s">
+        <v>30</v>
+      </c>
+      <c r="B328" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="s">
+        <v>47</v>
+      </c>
+      <c r="B329" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="s">
+        <v>26</v>
+      </c>
+      <c r="B330" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="s">
+        <v>40</v>
+      </c>
+      <c r="B331" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="s">
+        <v>85</v>
+      </c>
+      <c r="B332" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="s">
+        <v>159</v>
+      </c>
+      <c r="B333" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="s">
+        <v>71</v>
+      </c>
+      <c r="B334" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="s">
+        <v>69</v>
+      </c>
+      <c r="B335" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2238,25 +4114,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3146B8A8-4341-4398-9C19-AD3A37075BC7}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="52.28515625" customWidth="1"/>
-    <col min="7" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="68.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2283,7 +4159,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -2306,7 +4182,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2332,7 +4208,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2358,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -2381,7 +4257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2404,7 +4280,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2430,7 +4306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2456,7 +4332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -2479,7 +4355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -2505,7 +4381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2531,7 +4407,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -2554,7 +4430,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2577,7 +4453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -2603,7 +4479,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2629,7 +4505,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2655,7 +4531,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -2681,7 +4557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -2707,7 +4583,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -2733,7 +4609,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2762,7 +4638,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2791,7 +4667,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2811,7 +4687,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -2831,7 +4707,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2851,7 +4727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -2871,7 +4747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -2891,7 +4767,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -2911,7 +4787,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -2931,7 +4807,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -2951,7 +4827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -2971,7 +4847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -2991,7 +4867,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -3011,7 +4887,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -3031,7 +4907,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -3051,7 +4927,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -3074,7 +4950,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -3091,7 +4967,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -3111,7 +4987,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -3128,7 +5004,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -3145,7 +5021,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>89</v>
       </c>
@@ -3165,7 +5041,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -3185,7 +5061,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -3202,7 +5078,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -3219,7 +5095,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -3239,7 +5115,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -3259,7 +5135,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -3279,7 +5155,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>93</v>
       </c>
@@ -3299,7 +5175,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -3319,7 +5195,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>95</v>
       </c>
@@ -3339,7 +5215,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -3359,7 +5235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -3379,7 +5255,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>99</v>
       </c>
@@ -3399,7 +5275,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>158</v>
       </c>
@@ -3419,7 +5295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>156</v>
       </c>
@@ -3439,7 +5315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>155</v>
       </c>
@@ -3459,7 +5335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -3479,7 +5355,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>152</v>
       </c>
@@ -3496,7 +5372,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>154</v>
       </c>
@@ -3513,7 +5389,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>157</v>
       </c>
@@ -3559,7 +5435,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A62:A250 A2:A60</xm:sqref>
+          <xm:sqref>A2:A60 A62:A250</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
new req group for dynamics
</commit_message>
<xml_diff>
--- a/assets/i9sa.xlsx
+++ b/assets/i9sa.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9-esa/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EF22D6-130F-A244-9E0F-18AA85D266DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref" sheetId="2" r:id="rId1"/>
     <sheet name="Main" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName hidden="true" localSheetId="1" name="_xlnm._FilterDatabase">Main!$A$1:$F$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Main!$A$1:$F$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="192">
   <si>
     <t>Name</t>
   </si>
@@ -564,13 +565,64 @@
   </si>
   <si>
     <t>667cd55d52e83b24dbfe229e</t>
+  </si>
+  <si>
+    <t>Left Calf</t>
+  </si>
+  <si>
+    <t>Right Calf</t>
+  </si>
+  <si>
+    <t>Left Quad</t>
+  </si>
+  <si>
+    <t>Right Quad</t>
+  </si>
+  <si>
+    <t>Left Hamstring</t>
+  </si>
+  <si>
+    <t>Right Hamstring</t>
+  </si>
+  <si>
+    <t>Upper Back</t>
+  </si>
+  <si>
+    <t>Lower Back</t>
+  </si>
+  <si>
+    <t>Left Bicep</t>
+  </si>
+  <si>
+    <t>Right Bicep</t>
+  </si>
+  <si>
+    <t>Left Tricep</t>
+  </si>
+  <si>
+    <t>Right Tricep</t>
+  </si>
+  <si>
+    <t>Left Shoulder</t>
+  </si>
+  <si>
+    <t>Right Shoulder</t>
+  </si>
+  <si>
+    <t>Left Hip</t>
+  </si>
+  <si>
+    <t>Right Hip</t>
+  </si>
+  <si>
+    <t>Requirement Group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,7 +645,7 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -601,7 +653,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -609,7 +661,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -645,7 +697,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -653,7 +705,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -668,7 +720,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -683,7 +735,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i val="1"/>
+      <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -691,7 +743,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -755,19 +807,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999816888943144"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999938962981048"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3999755851924192"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -778,19 +830,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.7999816888943144"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.5999938962981048"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -801,19 +853,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.7999816888943144"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.5999938962981048"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.3999755851924192"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -824,19 +876,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999938962981048"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.3999755851924192"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -847,19 +899,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.7999816888943144"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.5999938962981048"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.3999755851924192"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -870,19 +922,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.7999816888943144"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.5999938962981048"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3999755851924192"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -918,7 +970,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.3999755851924192"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1005,97 +1057,97 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="true"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="true"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="true"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="true"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="true"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="true"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="true"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="true"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="true"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="true"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="true"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="true"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="true"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="true"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="true"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="true"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="true"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="true"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="true"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="true"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="true"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="true"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="true"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="true"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="true"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="true"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="true"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="true"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="true"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="true"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="true"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="true"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="true"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="true"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="true"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1103,8 +1155,18 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1117,154 +1179,154 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office 2013 - 2022 Theme">
-  <themeElements>
-    <clrScheme name="Office 2013 - 2022">
-      <dk1>
-        <sysClr val="windowText" lastClr="000000"/>
-      </dk1>
-      <lt1>
-        <sysClr val="window" lastClr="FFFFFF"/>
-      </lt1>
-      <dk2>
-        <srgbClr val="44546A"/>
-      </dk2>
-      <lt2>
-        <srgbClr val="E7E6E6"/>
-      </lt2>
-      <accent1>
-        <srgbClr val="4472C4"/>
-      </accent1>
-      <accent2>
-        <srgbClr val="ED7D31"/>
-      </accent2>
-      <accent3>
-        <srgbClr val="A5A5A5"/>
-      </accent3>
-      <accent4>
-        <srgbClr val="FFC000"/>
-      </accent4>
-      <accent5>
-        <srgbClr val="5B9BD5"/>
-      </accent5>
-      <accent6>
-        <srgbClr val="70AD47"/>
-      </accent6>
-      <hlink>
-        <srgbClr val="0563C1"/>
-      </hlink>
-      <folHlink>
-        <srgbClr val="954F72"/>
-      </folHlink>
-    </clrScheme>
-    <fontScheme name="Office 2013 - 2022">
-      <majorFont>
-        <latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <ea typeface=""/>
-        <cs typeface=""/>
-        <font script="Jpan" typeface="游ゴシック Light"/>
-        <font script="Hang" typeface="맑은 고딕"/>
-        <font script="Hans" typeface="等线 Light"/>
-        <font script="Hant" typeface="新細明體"/>
-        <font script="Arab" typeface="Times New Roman"/>
-        <font script="Hebr" typeface="Times New Roman"/>
-        <font script="Thai" typeface="Tahoma"/>
-        <font script="Ethi" typeface="Nyala"/>
-        <font script="Beng" typeface="Vrinda"/>
-        <font script="Gujr" typeface="Shruti"/>
-        <font script="Khmr" typeface="MoolBoran"/>
-        <font script="Knda" typeface="Tunga"/>
-        <font script="Guru" typeface="Raavi"/>
-        <font script="Cans" typeface="Euphemia"/>
-        <font script="Cher" typeface="Plantagenet Cherokee"/>
-        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <font script="Tibt" typeface="Microsoft Himalaya"/>
-        <font script="Thaa" typeface="MV Boli"/>
-        <font script="Deva" typeface="Mangal"/>
-        <font script="Telu" typeface="Gautami"/>
-        <font script="Taml" typeface="Latha"/>
-        <font script="Syrc" typeface="Estrangelo Edessa"/>
-        <font script="Orya" typeface="Kalinga"/>
-        <font script="Mlym" typeface="Kartika"/>
-        <font script="Laoo" typeface="DokChampa"/>
-        <font script="Sinh" typeface="Iskoola Pota"/>
-        <font script="Mong" typeface="Mongolian Baiti"/>
-        <font script="Viet" typeface="Times New Roman"/>
-        <font script="Uigh" typeface="Microsoft Uighur"/>
-        <font script="Geor" typeface="Sylfaen"/>
-        <font script="Armn" typeface="Arial"/>
-        <font script="Bugi" typeface="Leelawadee UI"/>
-        <font script="Bopo" typeface="Microsoft JhengHei"/>
-        <font script="Java" typeface="Javanese Text"/>
-        <font script="Lisu" typeface="Segoe UI"/>
-        <font script="Mymr" typeface="Myanmar Text"/>
-        <font script="Nkoo" typeface="Ebrima"/>
-        <font script="Olck" typeface="Nirmala UI"/>
-        <font script="Osma" typeface="Ebrima"/>
-        <font script="Phag" typeface="Phagspa"/>
-        <font script="Syrn" typeface="Estrangelo Edessa"/>
-        <font script="Syrj" typeface="Estrangelo Edessa"/>
-        <font script="Syre" typeface="Estrangelo Edessa"/>
-        <font script="Sora" typeface="Nirmala UI"/>
-        <font script="Tale" typeface="Microsoft Tai Le"/>
-        <font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <font script="Tfng" typeface="Ebrima"/>
-      </majorFont>
-      <minorFont>
-        <latin typeface="Calibri" panose="020F0502020204030204"/>
-        <ea typeface=""/>
-        <cs typeface=""/>
-        <font script="Jpan" typeface="游ゴシック"/>
-        <font script="Hang" typeface="맑은 고딕"/>
-        <font script="Hans" typeface="等线"/>
-        <font script="Hant" typeface="新細明體"/>
-        <font script="Arab" typeface="Arial"/>
-        <font script="Hebr" typeface="Arial"/>
-        <font script="Thai" typeface="Tahoma"/>
-        <font script="Ethi" typeface="Nyala"/>
-        <font script="Beng" typeface="Vrinda"/>
-        <font script="Gujr" typeface="Shruti"/>
-        <font script="Khmr" typeface="DaunPenh"/>
-        <font script="Knda" typeface="Tunga"/>
-        <font script="Guru" typeface="Raavi"/>
-        <font script="Cans" typeface="Euphemia"/>
-        <font script="Cher" typeface="Plantagenet Cherokee"/>
-        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <font script="Tibt" typeface="Microsoft Himalaya"/>
-        <font script="Thaa" typeface="MV Boli"/>
-        <font script="Deva" typeface="Mangal"/>
-        <font script="Telu" typeface="Gautami"/>
-        <font script="Taml" typeface="Latha"/>
-        <font script="Syrc" typeface="Estrangelo Edessa"/>
-        <font script="Orya" typeface="Kalinga"/>
-        <font script="Mlym" typeface="Kartika"/>
-        <font script="Laoo" typeface="DokChampa"/>
-        <font script="Sinh" typeface="Iskoola Pota"/>
-        <font script="Mong" typeface="Mongolian Baiti"/>
-        <font script="Viet" typeface="Arial"/>
-        <font script="Uigh" typeface="Microsoft Uighur"/>
-        <font script="Geor" typeface="Sylfaen"/>
-        <font script="Armn" typeface="Arial"/>
-        <font script="Bugi" typeface="Leelawadee UI"/>
-        <font script="Bopo" typeface="Microsoft JhengHei"/>
-        <font script="Java" typeface="Javanese Text"/>
-        <font script="Lisu" typeface="Segoe UI"/>
-        <font script="Mymr" typeface="Myanmar Text"/>
-        <font script="Nkoo" typeface="Ebrima"/>
-        <font script="Olck" typeface="Nirmala UI"/>
-        <font script="Osma" typeface="Ebrima"/>
-        <font script="Phag" typeface="Phagspa"/>
-        <font script="Syrn" typeface="Estrangelo Edessa"/>
-        <font script="Syrj" typeface="Estrangelo Edessa"/>
-        <font script="Syre" typeface="Estrangelo Edessa"/>
-        <font script="Sora" typeface="Nirmala UI"/>
-        <font script="Tale" typeface="Microsoft Tai Le"/>
-        <font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <font script="Tfng" typeface="Ebrima"/>
-      </minorFont>
-    </fontScheme>
-    <fmtScheme name="Office 2013 - 2022">
-      <fillStyleLst>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office 2013 - 2022">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office 2013 - 2022">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office 2013 - 2022">
+      <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1320,8 +1382,8 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </fillStyleLst>
-      <lnStyleLst>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1343,8 +1405,8 @@
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-      </lnStyleLst>
-      <effectStyleLst>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst/>
         </a:effectStyle>
@@ -1360,8 +1422,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-      </effectStyleLst>
-      <bgFillStyleLst>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1398,34 +1460,35 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </bgFillStyleLst>
-    </fmtScheme>
-  </themeElements>
-  <objectDefaults/>
-  <extraClrSchemeLst/>
-  <extLst>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
       <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
-  </extLst>
-</theme>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3FFC91-C2AA-49A2-9B33-E30FB4F3C11F}">
-  <dimension ref="A1:B103"/>
+  <dimension ref="A1:B335"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B152"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="true" customWidth="true" max="1" min="1" width="19.6640625"/>
-    <col bestFit="true" customWidth="true" max="2" min="2" width="26"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -1433,7 +1496,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1441,7 +1504,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1449,7 +1512,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1457,7 +1520,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -1465,7 +1528,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1473,7 +1536,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1481,7 +1544,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1489,7 +1552,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1497,7 +1560,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1505,7 +1568,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1513,7 +1576,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1521,7 +1584,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1529,7 +1592,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1537,7 +1600,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -1545,7 +1608,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1553,7 +1616,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1561,7 +1624,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1569,7 +1632,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -1577,7 +1640,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1585,7 +1648,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1593,7 +1656,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1601,7 +1664,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1609,7 +1672,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1617,7 +1680,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1625,7 +1688,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1633,7 +1696,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -1641,7 +1704,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -1649,7 +1712,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1657,7 +1720,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1665,7 +1728,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1673,7 +1736,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1681,7 +1744,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1689,7 +1752,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1697,7 +1760,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1705,7 +1768,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1713,7 +1776,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -1721,7 +1784,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -1729,7 +1792,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -1737,7 +1800,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1745,7 +1808,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1753,7 +1816,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1761,7 +1824,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -1769,7 +1832,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1777,7 +1840,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1785,7 +1848,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -1793,7 +1856,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -1801,7 +1864,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -1809,7 +1872,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -1817,7 +1880,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -1825,7 +1888,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>99</v>
       </c>
@@ -1833,7 +1896,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>81</v>
       </c>
@@ -1841,7 +1904,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>95</v>
       </c>
@@ -1849,7 +1912,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1857,7 +1920,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -1865,7 +1928,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>46</v>
       </c>
@@ -1873,7 +1936,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -1881,7 +1944,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>97</v>
       </c>
@@ -1889,7 +1952,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -1897,7 +1960,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -1905,7 +1968,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -1913,7 +1976,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>96</v>
       </c>
@@ -1921,7 +1984,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>91</v>
       </c>
@@ -1929,7 +1992,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -1937,7 +2000,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>85</v>
       </c>
@@ -1945,7 +2008,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>51</v>
       </c>
@@ -1953,7 +2016,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>44</v>
       </c>
@@ -1961,7 +2024,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -1969,7 +2032,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -1977,7 +2040,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -1985,7 +2048,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>94</v>
       </c>
@@ -1993,7 +2056,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>30</v>
       </c>
@@ -2001,7 +2064,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>31</v>
       </c>
@@ -2009,7 +2072,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>36</v>
       </c>
@@ -2017,7 +2080,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -2025,7 +2088,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>45</v>
       </c>
@@ -2033,7 +2096,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2041,7 +2104,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>37</v>
       </c>
@@ -2049,7 +2112,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>53</v>
       </c>
@@ -2057,7 +2120,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -2065,7 +2128,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>28</v>
       </c>
@@ -2073,7 +2136,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>35</v>
       </c>
@@ -2081,7 +2144,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -2089,7 +2152,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -2097,7 +2160,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>27</v>
       </c>
@@ -2105,7 +2168,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -2113,7 +2176,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>29</v>
       </c>
@@ -2121,7 +2184,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>32</v>
       </c>
@@ -2129,7 +2192,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>33</v>
       </c>
@@ -2137,7 +2200,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>38</v>
       </c>
@@ -2145,7 +2208,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>52</v>
       </c>
@@ -2153,7 +2216,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>41</v>
       </c>
@@ -2161,7 +2224,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -2169,7 +2232,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>34</v>
       </c>
@@ -2177,7 +2240,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>43</v>
       </c>
@@ -2185,7 +2248,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -2193,7 +2256,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>81</v>
       </c>
@@ -2201,7 +2264,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>93</v>
       </c>
@@ -2209,7 +2272,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>26</v>
       </c>
@@ -2217,7 +2280,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -2225,7 +2288,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>40</v>
       </c>
@@ -2233,7 +2296,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>50</v>
       </c>
@@ -2241,7 +2304,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>75</v>
       </c>
@@ -2249,7 +2312,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>38</v>
       </c>
@@ -2257,7 +2320,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>40</v>
       </c>
@@ -2265,7 +2328,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>46</v>
       </c>
@@ -2273,7 +2336,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>50</v>
       </c>
@@ -2281,7 +2344,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>158</v>
       </c>
@@ -2289,7 +2352,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>156</v>
       </c>
@@ -2297,7 +2360,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>28</v>
       </c>
@@ -2305,7 +2368,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>30</v>
       </c>
@@ -2313,7 +2376,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>88</v>
       </c>
@@ -2321,7 +2384,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>34</v>
       </c>
@@ -2329,7 +2392,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>81</v>
       </c>
@@ -2337,7 +2400,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>33</v>
       </c>
@@ -2345,7 +2408,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>159</v>
       </c>
@@ -2353,7 +2416,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>90</v>
       </c>
@@ -2361,7 +2424,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>51</v>
       </c>
@@ -2369,7 +2432,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>89</v>
       </c>
@@ -2377,7 +2440,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>75</v>
       </c>
@@ -2385,7 +2448,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>87</v>
       </c>
@@ -2393,7 +2456,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>93</v>
       </c>
@@ -2401,7 +2464,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>157</v>
       </c>
@@ -2409,7 +2472,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>44</v>
       </c>
@@ -2417,7 +2480,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -2425,7 +2488,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>32</v>
       </c>
@@ -2433,7 +2496,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>79</v>
       </c>
@@ -2441,7 +2504,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>83</v>
       </c>
@@ -2449,7 +2512,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>36</v>
       </c>
@@ -2457,7 +2520,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>37</v>
       </c>
@@ -2465,7 +2528,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>95</v>
       </c>
@@ -2473,7 +2536,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>27</v>
       </c>
@@ -2481,7 +2544,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>47</v>
       </c>
@@ -2489,7 +2552,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>99</v>
       </c>
@@ -2497,7 +2560,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>82</v>
       </c>
@@ -2505,7 +2568,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>94</v>
       </c>
@@ -2513,7 +2576,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>85</v>
       </c>
@@ -2521,7 +2584,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>96</v>
       </c>
@@ -2529,7 +2592,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>26</v>
       </c>
@@ -2537,7 +2600,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>42</v>
       </c>
@@ -2545,7 +2608,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>53</v>
       </c>
@@ -2553,7 +2616,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>70</v>
       </c>
@@ -2561,7 +2624,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>154</v>
       </c>
@@ -2569,7 +2632,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>29</v>
       </c>
@@ -2577,7 +2640,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>49</v>
       </c>
@@ -2585,7 +2648,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>80</v>
       </c>
@@ -2593,7 +2656,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>91</v>
       </c>
@@ -2601,7 +2664,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>155</v>
       </c>
@@ -2609,7 +2672,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>35</v>
       </c>
@@ -2617,7 +2680,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>43</v>
       </c>
@@ -2625,7 +2688,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>66</v>
       </c>
@@ -2633,7 +2696,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>77</v>
       </c>
@@ -2641,7 +2704,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>31</v>
       </c>
@@ -2649,7 +2712,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>52</v>
       </c>
@@ -2657,7 +2720,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -2665,7 +2728,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>39</v>
       </c>
@@ -2673,7 +2736,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>69</v>
       </c>
@@ -2681,7 +2744,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>45</v>
       </c>
@@ -2689,7 +2752,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>97</v>
       </c>
@@ -2697,7 +2760,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>41</v>
       </c>
@@ -2705,7 +2768,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>71</v>
       </c>
@@ -2713,7 +2776,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>89</v>
       </c>
@@ -2721,7 +2784,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>91</v>
       </c>
@@ -2729,7 +2792,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>97</v>
       </c>
@@ -2737,7 +2800,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>159</v>
       </c>
@@ -2745,7 +2808,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>32</v>
       </c>
@@ -2753,7 +2816,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>31</v>
       </c>
@@ -2761,7 +2824,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>44</v>
       </c>
@@ -2769,7 +2832,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>85</v>
       </c>
@@ -2777,7 +2840,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>51</v>
       </c>
@@ -2785,7 +2848,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>46</v>
       </c>
@@ -2793,7 +2856,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>83</v>
       </c>
@@ -2801,7 +2864,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>152</v>
       </c>
@@ -2809,7 +2872,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>45</v>
       </c>
@@ -2817,7 +2880,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>47</v>
       </c>
@@ -2825,7 +2888,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>81</v>
       </c>
@@ -2833,7 +2896,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>79</v>
       </c>
@@ -2841,7 +2904,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>87</v>
       </c>
@@ -2849,7 +2912,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>96</v>
       </c>
@@ -2857,7 +2920,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>38</v>
       </c>
@@ -2865,7 +2928,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>71</v>
       </c>
@@ -2873,7 +2936,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -2881,7 +2944,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>154</v>
       </c>
@@ -2889,7 +2952,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>27</v>
       </c>
@@ -2897,7 +2960,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>43</v>
       </c>
@@ -2905,7 +2968,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>88</v>
       </c>
@@ -2913,7 +2976,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>99</v>
       </c>
@@ -2921,7 +2984,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>30</v>
       </c>
@@ -2929,7 +2992,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>70</v>
       </c>
@@ -2937,7 +3000,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>80</v>
       </c>
@@ -2945,7 +3008,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>29</v>
       </c>
@@ -2953,7 +3016,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>77</v>
       </c>
@@ -2961,7 +3024,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>53</v>
       </c>
@@ -2969,7 +3032,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>156</v>
       </c>
@@ -2977,7 +3040,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>66</v>
       </c>
@@ -2985,7 +3048,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>90</v>
       </c>
@@ -2993,7 +3056,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>33</v>
       </c>
@@ -3001,7 +3064,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>40</v>
       </c>
@@ -3009,7 +3072,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>49</v>
       </c>
@@ -3017,7 +3080,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>157</v>
       </c>
@@ -3025,7 +3088,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>34</v>
       </c>
@@ -3033,7 +3096,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>36</v>
       </c>
@@ -3041,7 +3104,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>94</v>
       </c>
@@ -3049,7 +3112,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>50</v>
       </c>
@@ -3057,7 +3120,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>75</v>
       </c>
@@ -3065,7 +3128,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>82</v>
       </c>
@@ -3073,7 +3136,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>158</v>
       </c>
@@ -3081,7 +3144,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>35</v>
       </c>
@@ -3089,7 +3152,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>69</v>
       </c>
@@ -3097,7 +3160,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>95</v>
       </c>
@@ -3105,7 +3168,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>26</v>
       </c>
@@ -3113,7 +3176,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>39</v>
       </c>
@@ -3121,7 +3184,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>155</v>
       </c>
@@ -3129,7 +3192,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>42</v>
       </c>
@@ -3137,7 +3200,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>52</v>
       </c>
@@ -3145,7 +3208,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>93</v>
       </c>
@@ -3153,7 +3216,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>28</v>
       </c>
@@ -3161,7 +3224,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>37</v>
       </c>
@@ -3169,7 +3232,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>41</v>
       </c>
@@ -3177,7 +3240,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>91</v>
       </c>
@@ -3185,7 +3248,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>88</v>
       </c>
@@ -3193,7 +3256,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>36</v>
       </c>
@@ -3201,7 +3264,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>45</v>
       </c>
@@ -3209,7 +3272,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>47</v>
       </c>
@@ -3217,7 +3280,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>83</v>
       </c>
@@ -3225,7 +3288,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>34</v>
       </c>
@@ -3233,7 +3296,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>51</v>
       </c>
@@ -3241,7 +3304,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>28</v>
       </c>
@@ -3249,7 +3312,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>31</v>
       </c>
@@ -3257,7 +3320,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>35</v>
       </c>
@@ -3265,7 +3328,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>49</v>
       </c>
@@ -3273,7 +3336,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>75</v>
       </c>
@@ -3281,7 +3344,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>96</v>
       </c>
@@ -3289,7 +3352,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="234">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>158</v>
       </c>
@@ -3297,7 +3360,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>32</v>
       </c>
@@ -3305,7 +3368,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="236">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>157</v>
       </c>
@@ -3313,7 +3376,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="237">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>154</v>
       </c>
@@ -3321,7 +3384,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="238">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>50</v>
       </c>
@@ -3329,7 +3392,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>66</v>
       </c>
@@ -3337,7 +3400,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="240">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>94</v>
       </c>
@@ -3345,7 +3408,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="241">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>155</v>
       </c>
@@ -3353,7 +3416,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>159</v>
       </c>
@@ -3361,7 +3424,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>38</v>
       </c>
@@ -3369,7 +3432,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="244">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>43</v>
       </c>
@@ -3377,7 +3440,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="245">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>48</v>
       </c>
@@ -3385,7 +3448,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="246">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>77</v>
       </c>
@@ -3393,7 +3456,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="247">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>97</v>
       </c>
@@ -3401,7 +3464,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="248">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>26</v>
       </c>
@@ -3409,7 +3472,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="249">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>44</v>
       </c>
@@ -3417,7 +3480,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="250">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>33</v>
       </c>
@@ -3425,7 +3488,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="251">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>40</v>
       </c>
@@ -3433,7 +3496,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="252">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>71</v>
       </c>
@@ -3441,7 +3504,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="253">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>80</v>
       </c>
@@ -3449,7 +3512,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="254">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>152</v>
       </c>
@@ -3457,7 +3520,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="255">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>37</v>
       </c>
@@ -3465,7 +3528,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="256">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>90</v>
       </c>
@@ -3473,7 +3536,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="257">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>79</v>
       </c>
@@ -3481,7 +3544,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="258">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>85</v>
       </c>
@@ -3489,7 +3552,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="259">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>87</v>
       </c>
@@ -3497,7 +3560,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="260">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>93</v>
       </c>
@@ -3505,7 +3568,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="261">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>41</v>
       </c>
@@ -3513,7 +3576,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="262">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>82</v>
       </c>
@@ -3521,7 +3584,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="263">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>81</v>
       </c>
@@ -3529,7 +3592,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="264">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>46</v>
       </c>
@@ -3537,7 +3600,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="265">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>52</v>
       </c>
@@ -3545,7 +3608,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="266">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>42</v>
       </c>
@@ -3553,7 +3616,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="267">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>53</v>
       </c>
@@ -3561,7 +3624,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="268">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>70</v>
       </c>
@@ -3569,7 +3632,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="269">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>95</v>
       </c>
@@ -3577,7 +3640,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="270">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>156</v>
       </c>
@@ -3585,7 +3648,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="271">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>39</v>
       </c>
@@ -3593,7 +3656,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="272">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>30</v>
       </c>
@@ -3601,7 +3664,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="273">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>69</v>
       </c>
@@ -3609,7 +3672,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="274">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>27</v>
       </c>
@@ -3617,7 +3680,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="275">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>29</v>
       </c>
@@ -3625,7 +3688,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="276">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>99</v>
       </c>
@@ -3633,7 +3696,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="277">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>89</v>
       </c>
@@ -3641,7 +3704,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="278">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>152</v>
       </c>
@@ -3649,7 +3712,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="279">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>51</v>
       </c>
@@ -3657,7 +3720,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="280">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>41</v>
       </c>
@@ -3665,7 +3728,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="281">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>46</v>
       </c>
@@ -3673,7 +3736,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="282">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>49</v>
       </c>
@@ -3681,7 +3744,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="283">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>70</v>
       </c>
@@ -3689,7 +3752,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="284">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>81</v>
       </c>
@@ -3697,7 +3760,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="285">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>37</v>
       </c>
@@ -3705,7 +3768,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="286">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>39</v>
       </c>
@@ -3713,7 +3776,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="287">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>44</v>
       </c>
@@ -3721,7 +3784,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="288">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>158</v>
       </c>
@@ -3729,7 +3792,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="289">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>83</v>
       </c>
@@ -3737,7 +3800,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="290">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>91</v>
       </c>
@@ -3745,7 +3808,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="291">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>96</v>
       </c>
@@ -3753,7 +3816,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="292">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>97</v>
       </c>
@@ -3761,7 +3824,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="293">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>82</v>
       </c>
@@ -3769,7 +3832,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="294">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>89</v>
       </c>
@@ -3777,7 +3840,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="295">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>155</v>
       </c>
@@ -3785,7 +3848,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="296">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>154</v>
       </c>
@@ -3793,7 +3856,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="297">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>28</v>
       </c>
@@ -3801,7 +3864,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="298">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>75</v>
       </c>
@@ -3809,7 +3872,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="299">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>79</v>
       </c>
@@ -3817,7 +3880,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="300">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>87</v>
       </c>
@@ -3825,7 +3888,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="301">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>29</v>
       </c>
@@ -3833,7 +3896,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="302">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>50</v>
       </c>
@@ -3841,7 +3904,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="303">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>66</v>
       </c>
@@ -3849,7 +3912,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="304">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>88</v>
       </c>
@@ -3857,7 +3920,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="305">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>52</v>
       </c>
@@ -3865,7 +3928,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="306">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>53</v>
       </c>
@@ -3873,7 +3936,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="307">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>156</v>
       </c>
@@ -3881,7 +3944,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="308">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>157</v>
       </c>
@@ -3889,7 +3952,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="309">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>95</v>
       </c>
@@ -3897,7 +3960,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="310">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>99</v>
       </c>
@@ -3905,7 +3968,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="311">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>35</v>
       </c>
@@ -3913,7 +3976,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="312">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>36</v>
       </c>
@@ -3921,7 +3984,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="313">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>43</v>
       </c>
@@ -3929,7 +3992,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="314">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>94</v>
       </c>
@@ -3937,7 +4000,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="315">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>31</v>
       </c>
@@ -3945,7 +4008,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="316">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>34</v>
       </c>
@@ -3953,7 +4016,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="317">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>42</v>
       </c>
@@ -3961,7 +4024,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="318">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>32</v>
       </c>
@@ -3969,7 +4032,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="319">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>33</v>
       </c>
@@ -3977,7 +4040,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="320">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>90</v>
       </c>
@@ -3985,7 +4048,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="321">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>93</v>
       </c>
@@ -3993,7 +4056,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="322">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>38</v>
       </c>
@@ -4001,7 +4064,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="323">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>45</v>
       </c>
@@ -4009,7 +4072,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="324">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>48</v>
       </c>
@@ -4017,7 +4080,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="325">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>77</v>
       </c>
@@ -4025,7 +4088,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="326">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>80</v>
       </c>
@@ -4033,7 +4096,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="327">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>27</v>
       </c>
@@ -4041,7 +4104,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="328">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>30</v>
       </c>
@@ -4049,7 +4112,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="329">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>47</v>
       </c>
@@ -4057,7 +4120,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="330">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>26</v>
       </c>
@@ -4065,7 +4128,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="331">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>40</v>
       </c>
@@ -4073,7 +4136,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="332">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>85</v>
       </c>
@@ -4081,7 +4144,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="333">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>159</v>
       </c>
@@ -4089,7 +4152,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="334">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>71</v>
       </c>
@@ -4097,7 +4160,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="335">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>69</v>
       </c>
@@ -4106,16 +4169,20 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3146B8A8-4341-4398-9C19-AD3A37075BC7}">
-  <dimension ref="A1:J59"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4126,13 +4193,14 @@
     <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" customWidth="1"/>
     <col min="6" max="6" width="68.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" customWidth="1"/>
     <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4154,12 +4222,15 @@
       <c r="G1" t="s">
         <v>167</v>
       </c>
+      <c r="H1" t="s">
+        <v>191</v>
+      </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -4181,8 +4252,11 @@
       <c r="J2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -4207,8 +4281,11 @@
       <c r="J3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -4233,8 +4310,11 @@
       <c r="J4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -4256,8 +4336,11 @@
       <c r="J5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -4279,8 +4362,11 @@
       <c r="J6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -4305,8 +4391,11 @@
       <c r="J7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -4331,8 +4420,11 @@
       <c r="J8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -4354,8 +4446,11 @@
       <c r="J9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -4380,8 +4475,11 @@
       <c r="J10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -4406,8 +4504,11 @@
       <c r="J11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -4429,8 +4530,11 @@
       <c r="J12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -4452,8 +4556,11 @@
       <c r="J13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -4478,8 +4585,11 @@
       <c r="J14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -4504,8 +4614,11 @@
       <c r="J15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -4530,8 +4643,11 @@
       <c r="J16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -4556,8 +4672,11 @@
       <c r="J17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -4576,14 +4695,20 @@
       <c r="G18">
         <v>40</v>
       </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
       <c r="I18">
         <v>17</v>
       </c>
       <c r="J18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -4602,14 +4727,20 @@
       <c r="G19">
         <v>20</v>
       </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
       <c r="I19">
         <v>18</v>
       </c>
       <c r="J19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -4637,8 +4768,11 @@
       <c r="J20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -4666,8 +4800,11 @@
       <c r="J21" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -4687,7 +4824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -4707,7 +4844,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -4727,7 +4864,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -4746,8 +4883,11 @@
       <c r="G25">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -4767,7 +4907,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -4787,7 +4927,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -4807,7 +4947,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -4826,8 +4966,11 @@
       <c r="G29">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -4847,7 +4990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -4867,7 +5010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -4907,7 +5050,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -4950,7 +5093,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -4987,7 +5130,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -5004,7 +5147,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -5021,7 +5164,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>89</v>
       </c>
@@ -5041,7 +5184,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -5061,7 +5204,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -5078,7 +5221,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -5195,7 +5338,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>95</v>
       </c>
@@ -5215,7 +5358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -5235,7 +5378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -5255,7 +5398,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>99</v>
       </c>
@@ -5275,7 +5418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>158</v>
       </c>
@@ -5295,7 +5438,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>156</v>
       </c>
@@ -5314,13 +5457,16 @@
       <c r="G54">
         <v>40</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>155</v>
       </c>
       <c r="B55">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
@@ -5335,7 +5481,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -5355,7 +5501,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>152</v>
       </c>
@@ -5372,7 +5518,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>154</v>
       </c>
@@ -5389,7 +5535,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>157</v>
       </c>
@@ -5410,7 +5556,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F59" xr:uid="{3146B8A8-4341-4398-9C19-AD3A37075BC7}"/>
+  <autoFilter ref="A1:F59" xr:uid="{3146B8A8-4341-4398-9C19-AD3A37075BC7}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Dynamic"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="I1:J1"/>
   </mergeCells>

</xml_diff>

<commit_message>
whoops wrong col reqgroup
</commit_message>
<xml_diff>
--- a/assets/i9sa.xlsx
+++ b/assets/i9sa.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9-esa/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AD15DC-C38E-9849-80DA-BFB7F89E0C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ref" sheetId="2" r:id="rId1"/>
     <sheet name="Main" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Main!$A$1:$F$59</definedName>
+    <definedName hidden="true" localSheetId="1" name="_xlnm._FilterDatabase">Main!$A$1:$F$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -621,8 +620,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,7 +644,7 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -653,7 +652,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -661,7 +660,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -697,7 +696,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -705,7 +704,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -720,7 +719,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -735,7 +734,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <i val="1"/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -743,7 +742,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -807,19 +806,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -830,19 +829,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -853,19 +852,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -876,19 +875,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -899,19 +898,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -922,19 +921,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -970,7 +969,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.3999755851924192"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1057,95 +1056,95 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="true"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="true"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="true"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="true"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="true"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="true"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="true"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="true"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="true"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="true"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="true"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="true"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="true"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="true"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="true"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="true"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="true"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="true"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="true"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="true"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="true"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="true"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="true"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="true"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="true"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="true"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="true"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="true"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="true"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="true"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="true"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="true"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="true"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="true"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="true"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1166,7 +1165,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1179,154 +1178,154 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
-      <a:fillStyleLst>
+<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office 2013 - 2022 Theme">
+  <themeElements>
+    <clrScheme name="Office 2013 - 2022">
+      <dk1>
+        <sysClr val="windowText" lastClr="000000"/>
+      </dk1>
+      <lt1>
+        <sysClr val="window" lastClr="FFFFFF"/>
+      </lt1>
+      <dk2>
+        <srgbClr val="44546A"/>
+      </dk2>
+      <lt2>
+        <srgbClr val="E7E6E6"/>
+      </lt2>
+      <accent1>
+        <srgbClr val="4472C4"/>
+      </accent1>
+      <accent2>
+        <srgbClr val="ED7D31"/>
+      </accent2>
+      <accent3>
+        <srgbClr val="A5A5A5"/>
+      </accent3>
+      <accent4>
+        <srgbClr val="FFC000"/>
+      </accent4>
+      <accent5>
+        <srgbClr val="5B9BD5"/>
+      </accent5>
+      <accent6>
+        <srgbClr val="70AD47"/>
+      </accent6>
+      <hlink>
+        <srgbClr val="0563C1"/>
+      </hlink>
+      <folHlink>
+        <srgbClr val="954F72"/>
+      </folHlink>
+    </clrScheme>
+    <fontScheme name="Office 2013 - 2022">
+      <majorFont>
+        <latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="游ゴシック Light"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线 Light"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Times New Roman"/>
+        <font script="Hebr" typeface="Times New Roman"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="MoolBoran"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Times New Roman"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+        <font script="Armn" typeface="Arial"/>
+        <font script="Bugi" typeface="Leelawadee UI"/>
+        <font script="Bopo" typeface="Microsoft JhengHei"/>
+        <font script="Java" typeface="Javanese Text"/>
+        <font script="Lisu" typeface="Segoe UI"/>
+        <font script="Mymr" typeface="Myanmar Text"/>
+        <font script="Nkoo" typeface="Ebrima"/>
+        <font script="Olck" typeface="Nirmala UI"/>
+        <font script="Osma" typeface="Ebrima"/>
+        <font script="Phag" typeface="Phagspa"/>
+        <font script="Syrn" typeface="Estrangelo Edessa"/>
+        <font script="Syrj" typeface="Estrangelo Edessa"/>
+        <font script="Syre" typeface="Estrangelo Edessa"/>
+        <font script="Sora" typeface="Nirmala UI"/>
+        <font script="Tale" typeface="Microsoft Tai Le"/>
+        <font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <font script="Tfng" typeface="Ebrima"/>
+      </majorFont>
+      <minorFont>
+        <latin typeface="Calibri" panose="020F0502020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="游ゴシック"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Arial"/>
+        <font script="Hebr" typeface="Arial"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="DaunPenh"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Arial"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+        <font script="Armn" typeface="Arial"/>
+        <font script="Bugi" typeface="Leelawadee UI"/>
+        <font script="Bopo" typeface="Microsoft JhengHei"/>
+        <font script="Java" typeface="Javanese Text"/>
+        <font script="Lisu" typeface="Segoe UI"/>
+        <font script="Mymr" typeface="Myanmar Text"/>
+        <font script="Nkoo" typeface="Ebrima"/>
+        <font script="Olck" typeface="Nirmala UI"/>
+        <font script="Osma" typeface="Ebrima"/>
+        <font script="Phag" typeface="Phagspa"/>
+        <font script="Syrn" typeface="Estrangelo Edessa"/>
+        <font script="Syrj" typeface="Estrangelo Edessa"/>
+        <font script="Syre" typeface="Estrangelo Edessa"/>
+        <font script="Sora" typeface="Nirmala UI"/>
+        <font script="Tale" typeface="Microsoft Tai Le"/>
+        <font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <font script="Tfng" typeface="Ebrima"/>
+      </minorFont>
+    </fontScheme>
+    <fmtScheme name="Office 2013 - 2022">
+      <fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1382,8 +1381,8 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
+      </fillStyleLst>
+      <lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1405,8 +1404,8 @@
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
+      </lnStyleLst>
+      <effectStyleLst>
         <a:effectStyle>
           <a:effectLst/>
         </a:effectStyle>
@@ -1422,8 +1421,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
+      </effectStyleLst>
+      <bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1460,17 +1459,17 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
+      </bgFillStyleLst>
+    </fmtScheme>
+  </themeElements>
+  <objectDefaults/>
+  <extraClrSchemeLst/>
+  <extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
       <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
-  </a:extLst>
-</a:theme>
+  </extLst>
+</theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1481,14 +1480,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col bestFit="true" customWidth="true" max="1" min="1" width="19.6640625"/>
+    <col bestFit="true" customWidth="true" max="2" min="2" width="26"/>
+    <col bestFit="true" customWidth="true" max="4" min="4" width="24.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -1496,7 +1495,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1504,7 +1503,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1512,7 +1511,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1520,7 +1519,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -1528,7 +1527,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1536,7 +1535,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1544,7 +1543,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1552,7 +1551,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1560,7 +1559,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1568,7 +1567,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1576,7 +1575,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1584,7 +1583,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1592,7 +1591,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1600,7 +1599,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -1608,7 +1607,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1616,7 +1615,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1624,7 +1623,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1632,7 +1631,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -1640,7 +1639,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1648,7 +1647,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1656,7 +1655,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1664,7 +1663,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1672,7 +1671,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1680,7 +1679,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1696,7 +1695,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -1704,7 +1703,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -1712,7 +1711,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1720,7 +1719,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1728,7 +1727,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1736,7 +1735,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1744,7 +1743,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1752,7 +1751,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1760,7 +1759,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1768,7 +1767,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1776,7 +1775,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -1784,7 +1783,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -1792,7 +1791,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -1800,7 +1799,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1808,7 +1807,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1816,7 +1815,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -1832,7 +1831,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1840,7 +1839,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1848,7 +1847,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -1856,7 +1855,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -1864,7 +1863,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -1872,7 +1871,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -1880,7 +1879,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -1888,7 +1887,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>99</v>
       </c>
@@ -1896,7 +1895,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>81</v>
       </c>
@@ -1904,7 +1903,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>95</v>
       </c>
@@ -1912,7 +1911,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1920,7 +1919,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -1928,7 +1927,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>46</v>
       </c>
@@ -1936,7 +1935,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -1944,7 +1943,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>97</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -1968,7 +1967,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -1976,7 +1975,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>96</v>
       </c>
@@ -1984,7 +1983,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>91</v>
       </c>
@@ -1992,7 +1991,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -2000,7 +1999,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>85</v>
       </c>
@@ -2008,7 +2007,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>51</v>
       </c>
@@ -2016,7 +2015,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>44</v>
       </c>
@@ -2024,7 +2023,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -2032,7 +2031,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -2040,7 +2039,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -2048,7 +2047,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>94</v>
       </c>
@@ -2056,7 +2055,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>30</v>
       </c>
@@ -2064,7 +2063,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>31</v>
       </c>
@@ -2072,7 +2071,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>36</v>
       </c>
@@ -2080,7 +2079,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>45</v>
       </c>
@@ -2096,7 +2095,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2104,7 +2103,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>37</v>
       </c>
@@ -2112,7 +2111,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>53</v>
       </c>
@@ -2120,7 +2119,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -2128,7 +2127,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>28</v>
       </c>
@@ -2136,7 +2135,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>35</v>
       </c>
@@ -2144,7 +2143,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -2152,7 +2151,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -2160,7 +2159,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>27</v>
       </c>
@@ -2168,7 +2167,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -2176,7 +2175,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>29</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>32</v>
       </c>
@@ -2192,7 +2191,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>33</v>
       </c>
@@ -2200,7 +2199,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>38</v>
       </c>
@@ -2208,7 +2207,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>52</v>
       </c>
@@ -2216,7 +2215,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>41</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -2232,7 +2231,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>34</v>
       </c>
@@ -2240,7 +2239,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
         <v>43</v>
       </c>
@@ -2248,7 +2247,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -2256,7 +2255,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2">
       <c r="A97" t="s">
         <v>81</v>
       </c>
@@ -2264,7 +2263,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2">
       <c r="A98" t="s">
         <v>93</v>
       </c>
@@ -2272,7 +2271,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>26</v>
       </c>
@@ -2280,7 +2279,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -2288,7 +2287,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2">
       <c r="A101" t="s">
         <v>40</v>
       </c>
@@ -2296,7 +2295,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2">
       <c r="A102" t="s">
         <v>50</v>
       </c>
@@ -2304,7 +2303,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2">
       <c r="A103" t="s">
         <v>75</v>
       </c>
@@ -2312,7 +2311,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2">
       <c r="A104" t="s">
         <v>38</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2">
       <c r="A105" t="s">
         <v>40</v>
       </c>
@@ -2328,7 +2327,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2">
       <c r="A106" t="s">
         <v>46</v>
       </c>
@@ -2336,7 +2335,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2">
       <c r="A107" t="s">
         <v>50</v>
       </c>
@@ -2344,7 +2343,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2">
       <c r="A108" t="s">
         <v>158</v>
       </c>
@@ -2352,7 +2351,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2">
       <c r="A109" t="s">
         <v>156</v>
       </c>
@@ -2360,7 +2359,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2">
       <c r="A110" t="s">
         <v>28</v>
       </c>
@@ -2368,7 +2367,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2">
       <c r="A111" t="s">
         <v>30</v>
       </c>
@@ -2376,7 +2375,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2">
       <c r="A112" t="s">
         <v>88</v>
       </c>
@@ -2384,7 +2383,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2">
       <c r="A113" t="s">
         <v>34</v>
       </c>
@@ -2392,7 +2391,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2">
       <c r="A114" t="s">
         <v>81</v>
       </c>
@@ -2400,7 +2399,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2">
       <c r="A115" t="s">
         <v>33</v>
       </c>
@@ -2408,7 +2407,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2">
       <c r="A116" t="s">
         <v>159</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2">
       <c r="A117" t="s">
         <v>90</v>
       </c>
@@ -2424,7 +2423,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2">
       <c r="A118" t="s">
         <v>51</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2">
       <c r="A119" t="s">
         <v>89</v>
       </c>
@@ -2440,7 +2439,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2">
       <c r="A120" t="s">
         <v>75</v>
       </c>
@@ -2448,7 +2447,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2">
       <c r="A121" t="s">
         <v>87</v>
       </c>
@@ -2456,7 +2455,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2">
       <c r="A122" t="s">
         <v>93</v>
       </c>
@@ -2464,7 +2463,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2">
       <c r="A123" t="s">
         <v>157</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2">
       <c r="A124" t="s">
         <v>44</v>
       </c>
@@ -2480,7 +2479,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -2488,7 +2487,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2">
       <c r="A126" t="s">
         <v>32</v>
       </c>
@@ -2496,7 +2495,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2">
       <c r="A127" t="s">
         <v>79</v>
       </c>
@@ -2504,7 +2503,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2">
       <c r="A128" t="s">
         <v>83</v>
       </c>
@@ -2512,7 +2511,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2">
       <c r="A129" t="s">
         <v>36</v>
       </c>
@@ -2520,7 +2519,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2">
       <c r="A130" t="s">
         <v>37</v>
       </c>
@@ -2528,7 +2527,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2">
       <c r="A131" t="s">
         <v>95</v>
       </c>
@@ -2536,7 +2535,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2">
       <c r="A132" t="s">
         <v>27</v>
       </c>
@@ -2544,7 +2543,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2">
       <c r="A133" t="s">
         <v>47</v>
       </c>
@@ -2552,7 +2551,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2">
       <c r="A134" t="s">
         <v>99</v>
       </c>
@@ -2560,7 +2559,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2">
       <c r="A135" t="s">
         <v>82</v>
       </c>
@@ -2568,7 +2567,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2">
       <c r="A136" t="s">
         <v>94</v>
       </c>
@@ -2576,7 +2575,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2">
       <c r="A137" t="s">
         <v>85</v>
       </c>
@@ -2584,7 +2583,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2">
       <c r="A138" t="s">
         <v>96</v>
       </c>
@@ -2592,7 +2591,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2">
       <c r="A139" t="s">
         <v>26</v>
       </c>
@@ -2600,7 +2599,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2">
       <c r="A140" t="s">
         <v>42</v>
       </c>
@@ -2608,7 +2607,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2">
       <c r="A141" t="s">
         <v>53</v>
       </c>
@@ -2616,7 +2615,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2">
       <c r="A142" t="s">
         <v>70</v>
       </c>
@@ -2624,7 +2623,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2">
       <c r="A143" t="s">
         <v>154</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2">
       <c r="A144" t="s">
         <v>29</v>
       </c>
@@ -2640,7 +2639,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2">
       <c r="A145" t="s">
         <v>49</v>
       </c>
@@ -2648,7 +2647,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2">
       <c r="A146" t="s">
         <v>80</v>
       </c>
@@ -2656,7 +2655,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2">
       <c r="A147" t="s">
         <v>91</v>
       </c>
@@ -2664,7 +2663,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2">
       <c r="A148" t="s">
         <v>155</v>
       </c>
@@ -2672,7 +2671,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2">
       <c r="A149" t="s">
         <v>35</v>
       </c>
@@ -2680,7 +2679,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2">
       <c r="A150" t="s">
         <v>43</v>
       </c>
@@ -2688,7 +2687,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2">
       <c r="A151" t="s">
         <v>66</v>
       </c>
@@ -2696,7 +2695,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2">
       <c r="A152" t="s">
         <v>77</v>
       </c>
@@ -2704,7 +2703,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2">
       <c r="A153" t="s">
         <v>31</v>
       </c>
@@ -2712,7 +2711,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2">
       <c r="A154" t="s">
         <v>52</v>
       </c>
@@ -2720,7 +2719,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -2728,7 +2727,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2">
       <c r="A156" t="s">
         <v>39</v>
       </c>
@@ -2736,7 +2735,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2">
       <c r="A157" t="s">
         <v>69</v>
       </c>
@@ -2744,7 +2743,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2">
       <c r="A158" t="s">
         <v>45</v>
       </c>
@@ -2752,7 +2751,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2">
       <c r="A159" t="s">
         <v>97</v>
       </c>
@@ -2760,7 +2759,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2">
       <c r="A160" t="s">
         <v>41</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2">
       <c r="A161" t="s">
         <v>71</v>
       </c>
@@ -2776,7 +2775,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2">
       <c r="A162" t="s">
         <v>89</v>
       </c>
@@ -2784,7 +2783,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2">
       <c r="A163" t="s">
         <v>91</v>
       </c>
@@ -2792,7 +2791,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2">
       <c r="A164" t="s">
         <v>97</v>
       </c>
@@ -2800,7 +2799,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2">
       <c r="A165" t="s">
         <v>159</v>
       </c>
@@ -2808,7 +2807,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2">
       <c r="A166" t="s">
         <v>32</v>
       </c>
@@ -2816,7 +2815,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2">
       <c r="A167" t="s">
         <v>31</v>
       </c>
@@ -2824,7 +2823,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2">
       <c r="A168" t="s">
         <v>44</v>
       </c>
@@ -2832,7 +2831,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2">
       <c r="A169" t="s">
         <v>85</v>
       </c>
@@ -2840,7 +2839,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2">
       <c r="A170" t="s">
         <v>51</v>
       </c>
@@ -2848,7 +2847,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2">
       <c r="A171" t="s">
         <v>46</v>
       </c>
@@ -2856,7 +2855,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2">
       <c r="A172" t="s">
         <v>83</v>
       </c>
@@ -2864,7 +2863,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2">
       <c r="A173" t="s">
         <v>152</v>
       </c>
@@ -2872,7 +2871,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2">
       <c r="A174" t="s">
         <v>45</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2">
       <c r="A175" t="s">
         <v>47</v>
       </c>
@@ -2888,7 +2887,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2">
       <c r="A176" t="s">
         <v>81</v>
       </c>
@@ -2896,7 +2895,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2">
       <c r="A177" t="s">
         <v>79</v>
       </c>
@@ -2904,7 +2903,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2">
       <c r="A178" t="s">
         <v>87</v>
       </c>
@@ -2912,7 +2911,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2">
       <c r="A179" t="s">
         <v>96</v>
       </c>
@@ -2920,7 +2919,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2">
       <c r="A180" t="s">
         <v>38</v>
       </c>
@@ -2928,7 +2927,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2">
       <c r="A181" t="s">
         <v>71</v>
       </c>
@@ -2936,7 +2935,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -2944,7 +2943,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2">
       <c r="A183" t="s">
         <v>154</v>
       </c>
@@ -2952,7 +2951,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2">
       <c r="A184" t="s">
         <v>27</v>
       </c>
@@ -2960,7 +2959,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2">
       <c r="A185" t="s">
         <v>43</v>
       </c>
@@ -2968,7 +2967,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2">
       <c r="A186" t="s">
         <v>88</v>
       </c>
@@ -2976,7 +2975,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2">
       <c r="A187" t="s">
         <v>99</v>
       </c>
@@ -2984,7 +2983,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2">
       <c r="A188" t="s">
         <v>30</v>
       </c>
@@ -2992,7 +2991,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2">
       <c r="A189" t="s">
         <v>70</v>
       </c>
@@ -3000,7 +2999,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2">
       <c r="A190" t="s">
         <v>80</v>
       </c>
@@ -3008,7 +3007,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2">
       <c r="A191" t="s">
         <v>29</v>
       </c>
@@ -3016,7 +3015,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2">
       <c r="A192" t="s">
         <v>77</v>
       </c>
@@ -3024,7 +3023,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2">
       <c r="A193" t="s">
         <v>53</v>
       </c>
@@ -3032,7 +3031,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2">
       <c r="A194" t="s">
         <v>156</v>
       </c>
@@ -3040,7 +3039,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2">
       <c r="A195" t="s">
         <v>66</v>
       </c>
@@ -3048,7 +3047,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2">
       <c r="A196" t="s">
         <v>90</v>
       </c>
@@ -3056,7 +3055,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2">
       <c r="A197" t="s">
         <v>33</v>
       </c>
@@ -3064,7 +3063,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2">
       <c r="A198" t="s">
         <v>40</v>
       </c>
@@ -3072,7 +3071,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2">
       <c r="A199" t="s">
         <v>49</v>
       </c>
@@ -3080,7 +3079,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2">
       <c r="A200" t="s">
         <v>157</v>
       </c>
@@ -3088,7 +3087,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2">
       <c r="A201" t="s">
         <v>34</v>
       </c>
@@ -3096,7 +3095,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2">
       <c r="A202" t="s">
         <v>36</v>
       </c>
@@ -3104,7 +3103,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2">
       <c r="A203" t="s">
         <v>94</v>
       </c>
@@ -3112,7 +3111,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2">
       <c r="A204" t="s">
         <v>50</v>
       </c>
@@ -3120,7 +3119,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2">
       <c r="A205" t="s">
         <v>75</v>
       </c>
@@ -3128,7 +3127,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2">
       <c r="A206" t="s">
         <v>82</v>
       </c>
@@ -3136,7 +3135,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:2">
       <c r="A207" t="s">
         <v>158</v>
       </c>
@@ -3144,7 +3143,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2">
       <c r="A208" t="s">
         <v>35</v>
       </c>
@@ -3152,7 +3151,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:2">
       <c r="A209" t="s">
         <v>69</v>
       </c>
@@ -3160,7 +3159,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:2">
       <c r="A210" t="s">
         <v>95</v>
       </c>
@@ -3168,7 +3167,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:2">
       <c r="A211" t="s">
         <v>26</v>
       </c>
@@ -3176,7 +3175,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:2">
       <c r="A212" t="s">
         <v>39</v>
       </c>
@@ -3184,7 +3183,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:2">
       <c r="A213" t="s">
         <v>155</v>
       </c>
@@ -3192,7 +3191,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:2">
       <c r="A214" t="s">
         <v>42</v>
       </c>
@@ -3200,7 +3199,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:2">
       <c r="A215" t="s">
         <v>52</v>
       </c>
@@ -3208,7 +3207,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:2">
       <c r="A216" t="s">
         <v>93</v>
       </c>
@@ -3216,7 +3215,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:2">
       <c r="A217" t="s">
         <v>28</v>
       </c>
@@ -3224,7 +3223,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:2">
       <c r="A218" t="s">
         <v>37</v>
       </c>
@@ -3232,7 +3231,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:2">
       <c r="A219" t="s">
         <v>41</v>
       </c>
@@ -3240,7 +3239,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:2">
       <c r="A220" t="s">
         <v>91</v>
       </c>
@@ -3248,7 +3247,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:2">
       <c r="A221" t="s">
         <v>88</v>
       </c>
@@ -3256,7 +3255,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:2">
       <c r="A222" t="s">
         <v>36</v>
       </c>
@@ -3264,7 +3263,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:2">
       <c r="A223" t="s">
         <v>45</v>
       </c>
@@ -3272,7 +3271,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:2">
       <c r="A224" t="s">
         <v>47</v>
       </c>
@@ -3280,7 +3279,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:2">
       <c r="A225" t="s">
         <v>83</v>
       </c>
@@ -3288,7 +3287,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:2">
       <c r="A226" t="s">
         <v>34</v>
       </c>
@@ -3296,7 +3295,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:2">
       <c r="A227" t="s">
         <v>51</v>
       </c>
@@ -3304,7 +3303,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:2">
       <c r="A228" t="s">
         <v>28</v>
       </c>
@@ -3312,7 +3311,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:2">
       <c r="A229" t="s">
         <v>31</v>
       </c>
@@ -3320,7 +3319,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:2">
       <c r="A230" t="s">
         <v>35</v>
       </c>
@@ -3328,7 +3327,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:2">
       <c r="A231" t="s">
         <v>49</v>
       </c>
@@ -3336,7 +3335,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2">
       <c r="A232" t="s">
         <v>75</v>
       </c>
@@ -3344,7 +3343,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2">
       <c r="A233" t="s">
         <v>96</v>
       </c>
@@ -3352,7 +3351,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2">
       <c r="A234" t="s">
         <v>158</v>
       </c>
@@ -3360,7 +3359,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:2">
       <c r="A235" t="s">
         <v>32</v>
       </c>
@@ -3368,7 +3367,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:2">
       <c r="A236" t="s">
         <v>157</v>
       </c>
@@ -3376,7 +3375,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:2">
       <c r="A237" t="s">
         <v>154</v>
       </c>
@@ -3384,7 +3383,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:2">
       <c r="A238" t="s">
         <v>50</v>
       </c>
@@ -3392,7 +3391,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:2">
       <c r="A239" t="s">
         <v>66</v>
       </c>
@@ -3400,7 +3399,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:2">
       <c r="A240" t="s">
         <v>94</v>
       </c>
@@ -3408,7 +3407,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2">
       <c r="A241" t="s">
         <v>155</v>
       </c>
@@ -3416,7 +3415,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2">
       <c r="A242" t="s">
         <v>159</v>
       </c>
@@ -3424,7 +3423,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:2">
       <c r="A243" t="s">
         <v>38</v>
       </c>
@@ -3432,7 +3431,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:2">
       <c r="A244" t="s">
         <v>43</v>
       </c>
@@ -3440,7 +3439,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:2">
       <c r="A245" t="s">
         <v>48</v>
       </c>
@@ -3448,7 +3447,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:2">
       <c r="A246" t="s">
         <v>77</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:2">
       <c r="A247" t="s">
         <v>97</v>
       </c>
@@ -3464,7 +3463,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:2">
       <c r="A248" t="s">
         <v>26</v>
       </c>
@@ -3472,7 +3471,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:2">
       <c r="A249" t="s">
         <v>44</v>
       </c>
@@ -3480,7 +3479,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:2">
       <c r="A250" t="s">
         <v>33</v>
       </c>
@@ -3488,7 +3487,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:2">
       <c r="A251" t="s">
         <v>40</v>
       </c>
@@ -3496,7 +3495,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:2">
       <c r="A252" t="s">
         <v>71</v>
       </c>
@@ -3504,7 +3503,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:2">
       <c r="A253" t="s">
         <v>80</v>
       </c>
@@ -3512,7 +3511,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:2">
       <c r="A254" t="s">
         <v>152</v>
       </c>
@@ -3520,7 +3519,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:2">
       <c r="A255" t="s">
         <v>37</v>
       </c>
@@ -3528,7 +3527,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:2">
       <c r="A256" t="s">
         <v>90</v>
       </c>
@@ -3536,7 +3535,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:2">
       <c r="A257" t="s">
         <v>79</v>
       </c>
@@ -3544,7 +3543,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:2">
       <c r="A258" t="s">
         <v>85</v>
       </c>
@@ -3552,7 +3551,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:2">
       <c r="A259" t="s">
         <v>87</v>
       </c>
@@ -3560,7 +3559,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:2">
       <c r="A260" t="s">
         <v>93</v>
       </c>
@@ -3568,7 +3567,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:2">
       <c r="A261" t="s">
         <v>41</v>
       </c>
@@ -3576,7 +3575,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:2">
       <c r="A262" t="s">
         <v>82</v>
       </c>
@@ -3584,7 +3583,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:2">
       <c r="A263" t="s">
         <v>81</v>
       </c>
@@ -3592,7 +3591,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:2">
       <c r="A264" t="s">
         <v>46</v>
       </c>
@@ -3600,7 +3599,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:2">
       <c r="A265" t="s">
         <v>52</v>
       </c>
@@ -3608,7 +3607,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:2">
       <c r="A266" t="s">
         <v>42</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:2">
       <c r="A267" t="s">
         <v>53</v>
       </c>
@@ -3624,7 +3623,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:2">
       <c r="A268" t="s">
         <v>70</v>
       </c>
@@ -3632,7 +3631,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:2">
       <c r="A269" t="s">
         <v>95</v>
       </c>
@@ -3640,7 +3639,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:2">
       <c r="A270" t="s">
         <v>156</v>
       </c>
@@ -3648,7 +3647,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:2">
       <c r="A271" t="s">
         <v>39</v>
       </c>
@@ -3656,7 +3655,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:2">
       <c r="A272" t="s">
         <v>30</v>
       </c>
@@ -3664,7 +3663,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:2">
       <c r="A273" t="s">
         <v>69</v>
       </c>
@@ -3672,7 +3671,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:2">
       <c r="A274" t="s">
         <v>27</v>
       </c>
@@ -3680,7 +3679,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:2">
       <c r="A275" t="s">
         <v>29</v>
       </c>
@@ -3688,7 +3687,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:2">
       <c r="A276" t="s">
         <v>99</v>
       </c>
@@ -3696,7 +3695,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:2">
       <c r="A277" t="s">
         <v>89</v>
       </c>
@@ -3704,7 +3703,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:2">
       <c r="A278" t="s">
         <v>152</v>
       </c>
@@ -3712,7 +3711,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:2">
       <c r="A279" t="s">
         <v>51</v>
       </c>
@@ -3720,7 +3719,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:2">
       <c r="A280" t="s">
         <v>41</v>
       </c>
@@ -3728,7 +3727,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:2">
       <c r="A281" t="s">
         <v>46</v>
       </c>
@@ -3736,7 +3735,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:2">
       <c r="A282" t="s">
         <v>49</v>
       </c>
@@ -3744,7 +3743,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:2">
       <c r="A283" t="s">
         <v>70</v>
       </c>
@@ -3752,7 +3751,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:2">
       <c r="A284" t="s">
         <v>81</v>
       </c>
@@ -3760,7 +3759,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:2">
       <c r="A285" t="s">
         <v>37</v>
       </c>
@@ -3768,7 +3767,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:2">
       <c r="A286" t="s">
         <v>39</v>
       </c>
@@ -3776,7 +3775,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:2">
       <c r="A287" t="s">
         <v>44</v>
       </c>
@@ -3784,7 +3783,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:2">
       <c r="A288" t="s">
         <v>158</v>
       </c>
@@ -3792,7 +3791,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:2">
       <c r="A289" t="s">
         <v>83</v>
       </c>
@@ -3800,7 +3799,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:2">
       <c r="A290" t="s">
         <v>91</v>
       </c>
@@ -3808,7 +3807,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:2">
       <c r="A291" t="s">
         <v>96</v>
       </c>
@@ -3816,7 +3815,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:2">
       <c r="A292" t="s">
         <v>97</v>
       </c>
@@ -3824,7 +3823,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:2">
       <c r="A293" t="s">
         <v>82</v>
       </c>
@@ -3832,7 +3831,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:2">
       <c r="A294" t="s">
         <v>89</v>
       </c>
@@ -3840,7 +3839,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:2">
       <c r="A295" t="s">
         <v>155</v>
       </c>
@@ -3848,7 +3847,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:2">
       <c r="A296" t="s">
         <v>154</v>
       </c>
@@ -3856,7 +3855,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:2">
       <c r="A297" t="s">
         <v>28</v>
       </c>
@@ -3864,7 +3863,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:2">
       <c r="A298" t="s">
         <v>75</v>
       </c>
@@ -3872,7 +3871,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:2">
       <c r="A299" t="s">
         <v>79</v>
       </c>
@@ -3880,7 +3879,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:2">
       <c r="A300" t="s">
         <v>87</v>
       </c>
@@ -3888,7 +3887,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:2">
       <c r="A301" t="s">
         <v>29</v>
       </c>
@@ -3896,7 +3895,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:2">
       <c r="A302" t="s">
         <v>50</v>
       </c>
@@ -3904,7 +3903,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:2">
       <c r="A303" t="s">
         <v>66</v>
       </c>
@@ -3912,7 +3911,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:2">
       <c r="A304" t="s">
         <v>88</v>
       </c>
@@ -3920,7 +3919,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:2">
       <c r="A305" t="s">
         <v>52</v>
       </c>
@@ -3928,7 +3927,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:2">
       <c r="A306" t="s">
         <v>53</v>
       </c>
@@ -3936,7 +3935,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:2">
       <c r="A307" t="s">
         <v>156</v>
       </c>
@@ -3944,7 +3943,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:2">
       <c r="A308" t="s">
         <v>157</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:2">
       <c r="A309" t="s">
         <v>95</v>
       </c>
@@ -3960,7 +3959,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:2">
       <c r="A310" t="s">
         <v>99</v>
       </c>
@@ -3968,7 +3967,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:2">
       <c r="A311" t="s">
         <v>35</v>
       </c>
@@ -3976,7 +3975,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:2">
       <c r="A312" t="s">
         <v>36</v>
       </c>
@@ -3984,7 +3983,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:2">
       <c r="A313" t="s">
         <v>43</v>
       </c>
@@ -3992,7 +3991,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:2">
       <c r="A314" t="s">
         <v>94</v>
       </c>
@@ -4000,7 +3999,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:2">
       <c r="A315" t="s">
         <v>31</v>
       </c>
@@ -4008,7 +4007,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:2">
       <c r="A316" t="s">
         <v>34</v>
       </c>
@@ -4016,7 +4015,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:2">
       <c r="A317" t="s">
         <v>42</v>
       </c>
@@ -4024,7 +4023,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:2">
       <c r="A318" t="s">
         <v>32</v>
       </c>
@@ -4032,7 +4031,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:2">
       <c r="A319" t="s">
         <v>33</v>
       </c>
@@ -4040,7 +4039,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:2">
       <c r="A320" t="s">
         <v>90</v>
       </c>
@@ -4048,7 +4047,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:2">
       <c r="A321" t="s">
         <v>93</v>
       </c>
@@ -4056,7 +4055,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:2">
       <c r="A322" t="s">
         <v>38</v>
       </c>
@@ -4064,7 +4063,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:2">
       <c r="A323" t="s">
         <v>45</v>
       </c>
@@ -4072,7 +4071,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:2">
       <c r="A324" t="s">
         <v>48</v>
       </c>
@@ -4080,7 +4079,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:2">
       <c r="A325" t="s">
         <v>77</v>
       </c>
@@ -4088,7 +4087,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:2">
       <c r="A326" t="s">
         <v>80</v>
       </c>
@@ -4096,7 +4095,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:2">
       <c r="A327" t="s">
         <v>27</v>
       </c>
@@ -4104,7 +4103,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:2">
       <c r="A328" t="s">
         <v>30</v>
       </c>
@@ -4112,7 +4111,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:2">
       <c r="A329" t="s">
         <v>47</v>
       </c>
@@ -4120,7 +4119,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:2">
       <c r="A330" t="s">
         <v>26</v>
       </c>
@@ -4128,7 +4127,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:2">
       <c r="A331" t="s">
         <v>40</v>
       </c>
@@ -4136,7 +4135,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:2">
       <c r="A332" t="s">
         <v>85</v>
       </c>
@@ -4144,7 +4143,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:2">
       <c r="A333" t="s">
         <v>159</v>
       </c>
@@ -4152,7 +4151,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:2">
       <c r="A334" t="s">
         <v>71</v>
       </c>
@@ -4160,12 +4159,476 @@
         <v>134</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:2">
       <c r="A335" t="s">
         <v>69</v>
       </c>
       <c r="B335" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="s">
+        <v>66</v>
+      </c>
+      <c r="B336" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="s">
+        <v>80</v>
+      </c>
+      <c r="B337" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="s">
+        <v>28</v>
+      </c>
+      <c r="B338" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="s">
+        <v>38</v>
+      </c>
+      <c r="B339" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="s">
+        <v>42</v>
+      </c>
+      <c r="B340" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="s">
+        <v>43</v>
+      </c>
+      <c r="B341" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="s">
+        <v>79</v>
+      </c>
+      <c r="B342" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="s">
+        <v>88</v>
+      </c>
+      <c r="B343" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="s">
+        <v>158</v>
+      </c>
+      <c r="B344" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="s">
+        <v>32</v>
+      </c>
+      <c r="B345" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="s">
+        <v>31</v>
+      </c>
+      <c r="B346" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="s">
+        <v>69</v>
+      </c>
+      <c r="B347" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="s">
+        <v>91</v>
+      </c>
+      <c r="B348" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="s">
+        <v>89</v>
+      </c>
+      <c r="B349" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>87</v>
+      </c>
+      <c r="B350" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="s">
+        <v>52</v>
+      </c>
+      <c r="B351" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s">
+        <v>90</v>
+      </c>
+      <c r="B352" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="s">
+        <v>93</v>
+      </c>
+      <c r="B353" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="s">
+        <v>27</v>
+      </c>
+      <c r="B354" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="s">
+        <v>46</v>
+      </c>
+      <c r="B355" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="s">
+        <v>40</v>
+      </c>
+      <c r="B356" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="s">
+        <v>49</v>
+      </c>
+      <c r="B357" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="s">
+        <v>83</v>
+      </c>
+      <c r="B358" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="s">
+        <v>156</v>
+      </c>
+      <c r="B359" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="s">
+        <v>34</v>
+      </c>
+      <c r="B360" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="s">
+        <v>36</v>
+      </c>
+      <c r="B361" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="s">
+        <v>95</v>
+      </c>
+      <c r="B362" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="s">
+        <v>155</v>
+      </c>
+      <c r="B363" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="s">
+        <v>26</v>
+      </c>
+      <c r="B364" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="s">
+        <v>44</v>
+      </c>
+      <c r="B365" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="s">
+        <v>75</v>
+      </c>
+      <c r="B366" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="s">
+        <v>97</v>
+      </c>
+      <c r="B367" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="s">
+        <v>94</v>
+      </c>
+      <c r="B368" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="s">
+        <v>96</v>
+      </c>
+      <c r="B369" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="s">
+        <v>152</v>
+      </c>
+      <c r="B370" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="s">
+        <v>39</v>
+      </c>
+      <c r="B371" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="s">
+        <v>45</v>
+      </c>
+      <c r="B372" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="s">
+        <v>81</v>
+      </c>
+      <c r="B373" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="s">
+        <v>85</v>
+      </c>
+      <c r="B374" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="s">
+        <v>29</v>
+      </c>
+      <c r="B375" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="s">
+        <v>35</v>
+      </c>
+      <c r="B376" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="s">
+        <v>48</v>
+      </c>
+      <c r="B377" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="s">
+        <v>157</v>
+      </c>
+      <c r="B378" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="s">
+        <v>30</v>
+      </c>
+      <c r="B379" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="s">
+        <v>37</v>
+      </c>
+      <c r="B380" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="s">
+        <v>50</v>
+      </c>
+      <c r="B381" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="s">
+        <v>154</v>
+      </c>
+      <c r="B382" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="s">
+        <v>51</v>
+      </c>
+      <c r="B383" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="s">
+        <v>82</v>
+      </c>
+      <c r="B384" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="s">
+        <v>159</v>
+      </c>
+      <c r="B385" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="s">
+        <v>33</v>
+      </c>
+      <c r="B386" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="s">
+        <v>41</v>
+      </c>
+      <c r="B387" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="s">
+        <v>71</v>
+      </c>
+      <c r="B388" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="s">
+        <v>70</v>
+      </c>
+      <c r="B389" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="s">
+        <v>53</v>
+      </c>
+      <c r="B390" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="s">
+        <v>47</v>
+      </c>
+      <c r="B391" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="s">
+        <v>77</v>
+      </c>
+      <c r="B392" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="s">
+        <v>99</v>
+      </c>
+      <c r="B393" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify vals for new intro
</commit_message>
<xml_diff>
--- a/assets/i9sa.xlsx
+++ b/assets/i9sa.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9-esa/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF59CDCF-4A1E-4946-8988-E36234A735AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref" sheetId="2" r:id="rId1"/>
     <sheet name="Main" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName hidden="true" localSheetId="1" name="_xlnm._FilterDatabase">Main!$A$1:$F$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Main!$A$1:$F$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="192">
   <si>
     <t>Name</t>
   </si>
@@ -620,8 +621,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,7 +645,7 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -652,7 +653,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -660,7 +661,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -696,7 +697,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -704,7 +705,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -719,7 +720,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -734,7 +735,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i val="1"/>
+      <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -742,7 +743,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -806,19 +807,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999816888943144"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999938962981048"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3999755851924192"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -829,19 +830,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.7999816888943144"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.5999938962981048"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -852,19 +853,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.7999816888943144"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.5999938962981048"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.3999755851924192"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -875,19 +876,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999938962981048"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.3999755851924192"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -898,19 +899,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.7999816888943144"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.5999938962981048"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.3999755851924192"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -921,19 +922,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.7999816888943144"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.5999938962981048"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3999755851924192"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -969,7 +970,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.3999755851924192"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1056,95 +1057,95 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="true"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="true"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="true"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="true"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="true"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="true"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="true"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="true"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="true"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="true"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="true"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="true"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="true"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="true"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="true"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="true"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="true"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="true"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="true"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="true"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="true"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="true"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="true"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="true"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="true"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="true"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="true"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="true"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="true"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="true"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="true"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="true"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="true"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="true"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="true"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1165,7 +1166,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1178,154 +1179,154 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office 2013 - 2022 Theme">
-  <themeElements>
-    <clrScheme name="Office 2013 - 2022">
-      <dk1>
-        <sysClr val="windowText" lastClr="000000"/>
-      </dk1>
-      <lt1>
-        <sysClr val="window" lastClr="FFFFFF"/>
-      </lt1>
-      <dk2>
-        <srgbClr val="44546A"/>
-      </dk2>
-      <lt2>
-        <srgbClr val="E7E6E6"/>
-      </lt2>
-      <accent1>
-        <srgbClr val="4472C4"/>
-      </accent1>
-      <accent2>
-        <srgbClr val="ED7D31"/>
-      </accent2>
-      <accent3>
-        <srgbClr val="A5A5A5"/>
-      </accent3>
-      <accent4>
-        <srgbClr val="FFC000"/>
-      </accent4>
-      <accent5>
-        <srgbClr val="5B9BD5"/>
-      </accent5>
-      <accent6>
-        <srgbClr val="70AD47"/>
-      </accent6>
-      <hlink>
-        <srgbClr val="0563C1"/>
-      </hlink>
-      <folHlink>
-        <srgbClr val="954F72"/>
-      </folHlink>
-    </clrScheme>
-    <fontScheme name="Office 2013 - 2022">
-      <majorFont>
-        <latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <ea typeface=""/>
-        <cs typeface=""/>
-        <font script="Jpan" typeface="游ゴシック Light"/>
-        <font script="Hang" typeface="맑은 고딕"/>
-        <font script="Hans" typeface="等线 Light"/>
-        <font script="Hant" typeface="新細明體"/>
-        <font script="Arab" typeface="Times New Roman"/>
-        <font script="Hebr" typeface="Times New Roman"/>
-        <font script="Thai" typeface="Tahoma"/>
-        <font script="Ethi" typeface="Nyala"/>
-        <font script="Beng" typeface="Vrinda"/>
-        <font script="Gujr" typeface="Shruti"/>
-        <font script="Khmr" typeface="MoolBoran"/>
-        <font script="Knda" typeface="Tunga"/>
-        <font script="Guru" typeface="Raavi"/>
-        <font script="Cans" typeface="Euphemia"/>
-        <font script="Cher" typeface="Plantagenet Cherokee"/>
-        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <font script="Tibt" typeface="Microsoft Himalaya"/>
-        <font script="Thaa" typeface="MV Boli"/>
-        <font script="Deva" typeface="Mangal"/>
-        <font script="Telu" typeface="Gautami"/>
-        <font script="Taml" typeface="Latha"/>
-        <font script="Syrc" typeface="Estrangelo Edessa"/>
-        <font script="Orya" typeface="Kalinga"/>
-        <font script="Mlym" typeface="Kartika"/>
-        <font script="Laoo" typeface="DokChampa"/>
-        <font script="Sinh" typeface="Iskoola Pota"/>
-        <font script="Mong" typeface="Mongolian Baiti"/>
-        <font script="Viet" typeface="Times New Roman"/>
-        <font script="Uigh" typeface="Microsoft Uighur"/>
-        <font script="Geor" typeface="Sylfaen"/>
-        <font script="Armn" typeface="Arial"/>
-        <font script="Bugi" typeface="Leelawadee UI"/>
-        <font script="Bopo" typeface="Microsoft JhengHei"/>
-        <font script="Java" typeface="Javanese Text"/>
-        <font script="Lisu" typeface="Segoe UI"/>
-        <font script="Mymr" typeface="Myanmar Text"/>
-        <font script="Nkoo" typeface="Ebrima"/>
-        <font script="Olck" typeface="Nirmala UI"/>
-        <font script="Osma" typeface="Ebrima"/>
-        <font script="Phag" typeface="Phagspa"/>
-        <font script="Syrn" typeface="Estrangelo Edessa"/>
-        <font script="Syrj" typeface="Estrangelo Edessa"/>
-        <font script="Syre" typeface="Estrangelo Edessa"/>
-        <font script="Sora" typeface="Nirmala UI"/>
-        <font script="Tale" typeface="Microsoft Tai Le"/>
-        <font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <font script="Tfng" typeface="Ebrima"/>
-      </majorFont>
-      <minorFont>
-        <latin typeface="Calibri" panose="020F0502020204030204"/>
-        <ea typeface=""/>
-        <cs typeface=""/>
-        <font script="Jpan" typeface="游ゴシック"/>
-        <font script="Hang" typeface="맑은 고딕"/>
-        <font script="Hans" typeface="等线"/>
-        <font script="Hant" typeface="新細明體"/>
-        <font script="Arab" typeface="Arial"/>
-        <font script="Hebr" typeface="Arial"/>
-        <font script="Thai" typeface="Tahoma"/>
-        <font script="Ethi" typeface="Nyala"/>
-        <font script="Beng" typeface="Vrinda"/>
-        <font script="Gujr" typeface="Shruti"/>
-        <font script="Khmr" typeface="DaunPenh"/>
-        <font script="Knda" typeface="Tunga"/>
-        <font script="Guru" typeface="Raavi"/>
-        <font script="Cans" typeface="Euphemia"/>
-        <font script="Cher" typeface="Plantagenet Cherokee"/>
-        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <font script="Tibt" typeface="Microsoft Himalaya"/>
-        <font script="Thaa" typeface="MV Boli"/>
-        <font script="Deva" typeface="Mangal"/>
-        <font script="Telu" typeface="Gautami"/>
-        <font script="Taml" typeface="Latha"/>
-        <font script="Syrc" typeface="Estrangelo Edessa"/>
-        <font script="Orya" typeface="Kalinga"/>
-        <font script="Mlym" typeface="Kartika"/>
-        <font script="Laoo" typeface="DokChampa"/>
-        <font script="Sinh" typeface="Iskoola Pota"/>
-        <font script="Mong" typeface="Mongolian Baiti"/>
-        <font script="Viet" typeface="Arial"/>
-        <font script="Uigh" typeface="Microsoft Uighur"/>
-        <font script="Geor" typeface="Sylfaen"/>
-        <font script="Armn" typeface="Arial"/>
-        <font script="Bugi" typeface="Leelawadee UI"/>
-        <font script="Bopo" typeface="Microsoft JhengHei"/>
-        <font script="Java" typeface="Javanese Text"/>
-        <font script="Lisu" typeface="Segoe UI"/>
-        <font script="Mymr" typeface="Myanmar Text"/>
-        <font script="Nkoo" typeface="Ebrima"/>
-        <font script="Olck" typeface="Nirmala UI"/>
-        <font script="Osma" typeface="Ebrima"/>
-        <font script="Phag" typeface="Phagspa"/>
-        <font script="Syrn" typeface="Estrangelo Edessa"/>
-        <font script="Syrj" typeface="Estrangelo Edessa"/>
-        <font script="Syre" typeface="Estrangelo Edessa"/>
-        <font script="Sora" typeface="Nirmala UI"/>
-        <font script="Tale" typeface="Microsoft Tai Le"/>
-        <font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <font script="Tfng" typeface="Ebrima"/>
-      </minorFont>
-    </fontScheme>
-    <fmtScheme name="Office 2013 - 2022">
-      <fillStyleLst>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office 2013 - 2022">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office 2013 - 2022">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office 2013 - 2022">
+      <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1381,8 +1382,8 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </fillStyleLst>
-      <lnStyleLst>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1404,8 +1405,8 @@
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-      </lnStyleLst>
-      <effectStyleLst>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst/>
         </a:effectStyle>
@@ -1421,8 +1422,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-      </effectStyleLst>
-      <bgFillStyleLst>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1459,35 +1460,35 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </bgFillStyleLst>
-    </fmtScheme>
-  </themeElements>
-  <objectDefaults/>
-  <extraClrSchemeLst/>
-  <extLst>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
       <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
-  </extLst>
-</theme>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3FFC91-C2AA-49A2-9B33-E30FB4F3C11F}">
-  <dimension ref="A1:B335"/>
+  <dimension ref="A1:B451"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="true" customWidth="true" max="1" min="1" width="19.6640625"/>
-    <col bestFit="true" customWidth="true" max="2" min="2" width="26"/>
-    <col bestFit="true" customWidth="true" max="4" min="4" width="24.6640625"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -1495,7 +1496,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1503,7 +1504,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1511,7 +1512,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1519,7 +1520,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1543,7 +1544,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1551,7 +1552,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1559,7 +1560,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1567,7 +1568,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1583,7 +1584,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1591,7 +1592,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1599,7 +1600,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1623,7 +1624,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -1639,7 +1640,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1671,7 +1672,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -1711,7 +1712,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1719,7 +1720,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1735,7 +1736,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1759,7 +1760,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1767,7 +1768,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1775,7 +1776,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -1783,7 +1784,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -1791,7 +1792,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1815,7 +1816,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1823,7 +1824,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -1831,7 +1832,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1839,7 +1840,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -1863,7 +1864,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -1871,7 +1872,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -1879,7 +1880,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>99</v>
       </c>
@@ -1895,7 +1896,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>81</v>
       </c>
@@ -1903,7 +1904,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>95</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1919,7 +1920,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>46</v>
       </c>
@@ -1935,7 +1936,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -1943,7 +1944,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>97</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -1959,7 +1960,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -1967,7 +1968,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -1975,7 +1976,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>96</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>91</v>
       </c>
@@ -1991,7 +1992,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -1999,7 +2000,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>85</v>
       </c>
@@ -2007,7 +2008,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>51</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>44</v>
       </c>
@@ -2023,7 +2024,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -2031,7 +2032,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -2039,7 +2040,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -2047,7 +2048,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>94</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>30</v>
       </c>
@@ -2063,7 +2064,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>31</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>36</v>
       </c>
@@ -2079,7 +2080,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -2087,7 +2088,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>45</v>
       </c>
@@ -2095,7 +2096,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2103,7 +2104,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>37</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>53</v>
       </c>
@@ -2119,7 +2120,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -2127,7 +2128,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>28</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>35</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -2151,7 +2152,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>27</v>
       </c>
@@ -2167,7 +2168,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -2175,7 +2176,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>29</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>32</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>33</v>
       </c>
@@ -2199,7 +2200,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>38</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>52</v>
       </c>
@@ -2215,7 +2216,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>41</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -2231,7 +2232,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>34</v>
       </c>
@@ -2239,7 +2240,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>43</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>81</v>
       </c>
@@ -2263,7 +2264,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>93</v>
       </c>
@@ -2271,7 +2272,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>26</v>
       </c>
@@ -2279,7 +2280,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -2287,7 +2288,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>40</v>
       </c>
@@ -2295,7 +2296,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>50</v>
       </c>
@@ -2303,7 +2304,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>75</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>38</v>
       </c>
@@ -2319,7 +2320,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>40</v>
       </c>
@@ -2327,7 +2328,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>46</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>50</v>
       </c>
@@ -2343,7 +2344,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>158</v>
       </c>
@@ -2351,7 +2352,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>156</v>
       </c>
@@ -2359,7 +2360,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>28</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>30</v>
       </c>
@@ -2375,7 +2376,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>88</v>
       </c>
@@ -2383,7 +2384,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>34</v>
       </c>
@@ -2391,7 +2392,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>81</v>
       </c>
@@ -2399,7 +2400,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>33</v>
       </c>
@@ -2407,7 +2408,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>159</v>
       </c>
@@ -2415,7 +2416,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>90</v>
       </c>
@@ -2423,7 +2424,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>51</v>
       </c>
@@ -2431,7 +2432,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>89</v>
       </c>
@@ -2439,7 +2440,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>75</v>
       </c>
@@ -2447,7 +2448,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>87</v>
       </c>
@@ -2455,7 +2456,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>93</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>157</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>44</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -2487,7 +2488,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>32</v>
       </c>
@@ -2495,7 +2496,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>79</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>83</v>
       </c>
@@ -2511,7 +2512,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>36</v>
       </c>
@@ -2519,7 +2520,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>37</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>95</v>
       </c>
@@ -2535,7 +2536,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>27</v>
       </c>
@@ -2543,7 +2544,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>47</v>
       </c>
@@ -2551,7 +2552,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>99</v>
       </c>
@@ -2559,7 +2560,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>82</v>
       </c>
@@ -2567,7 +2568,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>94</v>
       </c>
@@ -2575,7 +2576,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>85</v>
       </c>
@@ -2583,7 +2584,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>96</v>
       </c>
@@ -2591,7 +2592,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>26</v>
       </c>
@@ -2599,7 +2600,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>42</v>
       </c>
@@ -2607,7 +2608,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>53</v>
       </c>
@@ -2615,7 +2616,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>70</v>
       </c>
@@ -2623,7 +2624,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>154</v>
       </c>
@@ -2631,7 +2632,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>29</v>
       </c>
@@ -2639,7 +2640,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>49</v>
       </c>
@@ -2647,7 +2648,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>80</v>
       </c>
@@ -2655,7 +2656,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>91</v>
       </c>
@@ -2663,7 +2664,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>155</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>35</v>
       </c>
@@ -2679,7 +2680,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>43</v>
       </c>
@@ -2687,7 +2688,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>66</v>
       </c>
@@ -2695,7 +2696,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>77</v>
       </c>
@@ -2703,7 +2704,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>31</v>
       </c>
@@ -2711,7 +2712,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>52</v>
       </c>
@@ -2719,7 +2720,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -2727,7 +2728,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>39</v>
       </c>
@@ -2735,7 +2736,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>69</v>
       </c>
@@ -2743,7 +2744,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>45</v>
       </c>
@@ -2751,7 +2752,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>97</v>
       </c>
@@ -2759,7 +2760,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>41</v>
       </c>
@@ -2767,7 +2768,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>71</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>89</v>
       </c>
@@ -2783,7 +2784,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>91</v>
       </c>
@@ -2791,7 +2792,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>97</v>
       </c>
@@ -2799,7 +2800,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>159</v>
       </c>
@@ -2807,7 +2808,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>32</v>
       </c>
@@ -2815,7 +2816,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>31</v>
       </c>
@@ -2823,7 +2824,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>44</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>85</v>
       </c>
@@ -2839,7 +2840,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>51</v>
       </c>
@@ -2847,7 +2848,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>46</v>
       </c>
@@ -2855,7 +2856,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>83</v>
       </c>
@@ -2863,7 +2864,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>152</v>
       </c>
@@ -2871,7 +2872,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>45</v>
       </c>
@@ -2879,7 +2880,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>47</v>
       </c>
@@ -2887,7 +2888,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>81</v>
       </c>
@@ -2895,7 +2896,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>79</v>
       </c>
@@ -2903,7 +2904,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>87</v>
       </c>
@@ -2911,7 +2912,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>96</v>
       </c>
@@ -2919,7 +2920,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>38</v>
       </c>
@@ -2927,7 +2928,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>71</v>
       </c>
@@ -2935,7 +2936,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -2943,7 +2944,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>154</v>
       </c>
@@ -2951,7 +2952,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>27</v>
       </c>
@@ -2959,7 +2960,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>43</v>
       </c>
@@ -2967,7 +2968,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>88</v>
       </c>
@@ -2975,7 +2976,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>99</v>
       </c>
@@ -2983,7 +2984,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>30</v>
       </c>
@@ -2991,7 +2992,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>70</v>
       </c>
@@ -2999,7 +3000,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>80</v>
       </c>
@@ -3007,7 +3008,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>29</v>
       </c>
@@ -3015,7 +3016,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>77</v>
       </c>
@@ -3023,7 +3024,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>53</v>
       </c>
@@ -3031,7 +3032,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>156</v>
       </c>
@@ -3039,7 +3040,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>66</v>
       </c>
@@ -3047,7 +3048,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>90</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>33</v>
       </c>
@@ -3063,7 +3064,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>40</v>
       </c>
@@ -3071,7 +3072,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>49</v>
       </c>
@@ -3079,7 +3080,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>157</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>34</v>
       </c>
@@ -3095,7 +3096,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>36</v>
       </c>
@@ -3103,7 +3104,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>94</v>
       </c>
@@ -3111,7 +3112,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>50</v>
       </c>
@@ -3119,7 +3120,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>75</v>
       </c>
@@ -3127,7 +3128,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>82</v>
       </c>
@@ -3135,7 +3136,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>158</v>
       </c>
@@ -3143,7 +3144,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>35</v>
       </c>
@@ -3151,7 +3152,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>69</v>
       </c>
@@ -3159,7 +3160,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>95</v>
       </c>
@@ -3167,7 +3168,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>26</v>
       </c>
@@ -3175,7 +3176,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>39</v>
       </c>
@@ -3183,7 +3184,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>155</v>
       </c>
@@ -3191,7 +3192,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>42</v>
       </c>
@@ -3199,7 +3200,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>52</v>
       </c>
@@ -3207,7 +3208,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>93</v>
       </c>
@@ -3215,7 +3216,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>28</v>
       </c>
@@ -3223,7 +3224,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>37</v>
       </c>
@@ -3231,7 +3232,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>41</v>
       </c>
@@ -3239,7 +3240,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>91</v>
       </c>
@@ -3247,7 +3248,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>88</v>
       </c>
@@ -3255,7 +3256,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>36</v>
       </c>
@@ -3263,7 +3264,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>45</v>
       </c>
@@ -3271,7 +3272,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>47</v>
       </c>
@@ -3279,7 +3280,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>83</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>34</v>
       </c>
@@ -3295,7 +3296,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>51</v>
       </c>
@@ -3303,7 +3304,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>28</v>
       </c>
@@ -3311,7 +3312,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>31</v>
       </c>
@@ -3319,7 +3320,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>35</v>
       </c>
@@ -3327,7 +3328,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>49</v>
       </c>
@@ -3335,7 +3336,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>75</v>
       </c>
@@ -3343,7 +3344,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>96</v>
       </c>
@@ -3351,7 +3352,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>158</v>
       </c>
@@ -3359,7 +3360,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>32</v>
       </c>
@@ -3367,7 +3368,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>157</v>
       </c>
@@ -3375,7 +3376,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>154</v>
       </c>
@@ -3383,7 +3384,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>50</v>
       </c>
@@ -3391,7 +3392,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>66</v>
       </c>
@@ -3399,7 +3400,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>94</v>
       </c>
@@ -3407,7 +3408,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>155</v>
       </c>
@@ -3415,7 +3416,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>159</v>
       </c>
@@ -3423,7 +3424,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>38</v>
       </c>
@@ -3431,7 +3432,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>43</v>
       </c>
@@ -3439,7 +3440,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>48</v>
       </c>
@@ -3447,7 +3448,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>77</v>
       </c>
@@ -3455,7 +3456,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>97</v>
       </c>
@@ -3463,7 +3464,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>26</v>
       </c>
@@ -3471,7 +3472,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>44</v>
       </c>
@@ -3479,7 +3480,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>33</v>
       </c>
@@ -3487,7 +3488,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>40</v>
       </c>
@@ -3495,7 +3496,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>71</v>
       </c>
@@ -3503,7 +3504,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>80</v>
       </c>
@@ -3511,7 +3512,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>152</v>
       </c>
@@ -3519,7 +3520,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>37</v>
       </c>
@@ -3527,7 +3528,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>90</v>
       </c>
@@ -3535,7 +3536,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>79</v>
       </c>
@@ -3543,7 +3544,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>85</v>
       </c>
@@ -3551,7 +3552,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>87</v>
       </c>
@@ -3559,7 +3560,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>93</v>
       </c>
@@ -3567,7 +3568,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>41</v>
       </c>
@@ -3575,7 +3576,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>82</v>
       </c>
@@ -3583,7 +3584,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>81</v>
       </c>
@@ -3591,7 +3592,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>46</v>
       </c>
@@ -3599,7 +3600,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>52</v>
       </c>
@@ -3607,7 +3608,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>42</v>
       </c>
@@ -3615,7 +3616,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>53</v>
       </c>
@@ -3623,7 +3624,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>70</v>
       </c>
@@ -3631,7 +3632,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>95</v>
       </c>
@@ -3639,7 +3640,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>156</v>
       </c>
@@ -3647,7 +3648,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>39</v>
       </c>
@@ -3655,7 +3656,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>30</v>
       </c>
@@ -3663,7 +3664,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>69</v>
       </c>
@@ -3671,7 +3672,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>27</v>
       </c>
@@ -3679,7 +3680,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>29</v>
       </c>
@@ -3687,7 +3688,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>99</v>
       </c>
@@ -3695,7 +3696,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>89</v>
       </c>
@@ -3703,7 +3704,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>152</v>
       </c>
@@ -3711,7 +3712,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>51</v>
       </c>
@@ -3719,7 +3720,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>41</v>
       </c>
@@ -3727,7 +3728,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>46</v>
       </c>
@@ -3735,7 +3736,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>49</v>
       </c>
@@ -3743,7 +3744,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>70</v>
       </c>
@@ -3751,7 +3752,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>81</v>
       </c>
@@ -3759,7 +3760,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>37</v>
       </c>
@@ -3767,7 +3768,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>39</v>
       </c>
@@ -3775,7 +3776,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>44</v>
       </c>
@@ -3783,7 +3784,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>158</v>
       </c>
@@ -3791,7 +3792,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>83</v>
       </c>
@@ -3799,7 +3800,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>91</v>
       </c>
@@ -3807,7 +3808,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>96</v>
       </c>
@@ -3815,7 +3816,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>97</v>
       </c>
@@ -3823,7 +3824,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>82</v>
       </c>
@@ -3831,7 +3832,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>89</v>
       </c>
@@ -3839,7 +3840,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>155</v>
       </c>
@@ -3847,7 +3848,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>154</v>
       </c>
@@ -3855,7 +3856,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>28</v>
       </c>
@@ -3863,7 +3864,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>75</v>
       </c>
@@ -3871,7 +3872,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>79</v>
       </c>
@@ -3879,7 +3880,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>87</v>
       </c>
@@ -3887,7 +3888,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>29</v>
       </c>
@@ -3895,7 +3896,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>50</v>
       </c>
@@ -3903,7 +3904,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="303" spans="1:2">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>66</v>
       </c>
@@ -3911,7 +3912,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>88</v>
       </c>
@@ -3919,7 +3920,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="305" spans="1:2">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>52</v>
       </c>
@@ -3927,7 +3928,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="306" spans="1:2">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>53</v>
       </c>
@@ -3935,7 +3936,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="307" spans="1:2">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>156</v>
       </c>
@@ -3943,7 +3944,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="308" spans="1:2">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>157</v>
       </c>
@@ -3951,7 +3952,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="309" spans="1:2">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>95</v>
       </c>
@@ -3959,7 +3960,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="310" spans="1:2">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>99</v>
       </c>
@@ -3967,7 +3968,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="311" spans="1:2">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>35</v>
       </c>
@@ -3975,7 +3976,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="312" spans="1:2">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>36</v>
       </c>
@@ -3983,7 +3984,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="313" spans="1:2">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>43</v>
       </c>
@@ -3991,7 +3992,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="314" spans="1:2">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>94</v>
       </c>
@@ -3999,7 +4000,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="315" spans="1:2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>31</v>
       </c>
@@ -4007,7 +4008,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="316" spans="1:2">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>34</v>
       </c>
@@ -4015,7 +4016,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="317" spans="1:2">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>42</v>
       </c>
@@ -4023,7 +4024,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="318" spans="1:2">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>32</v>
       </c>
@@ -4031,7 +4032,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="319" spans="1:2">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>33</v>
       </c>
@@ -4039,7 +4040,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="320" spans="1:2">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>90</v>
       </c>
@@ -4047,7 +4048,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>93</v>
       </c>
@@ -4055,7 +4056,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>38</v>
       </c>
@@ -4063,7 +4064,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="323" spans="1:2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>45</v>
       </c>
@@ -4071,7 +4072,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>48</v>
       </c>
@@ -4079,7 +4080,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="325" spans="1:2">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>77</v>
       </c>
@@ -4087,7 +4088,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="326" spans="1:2">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>80</v>
       </c>
@@ -4095,7 +4096,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="327" spans="1:2">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>27</v>
       </c>
@@ -4103,7 +4104,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="328" spans="1:2">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>30</v>
       </c>
@@ -4111,7 +4112,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="329" spans="1:2">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>47</v>
       </c>
@@ -4119,7 +4120,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>26</v>
       </c>
@@ -4127,7 +4128,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="331" spans="1:2">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>40</v>
       </c>
@@ -4135,7 +4136,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>85</v>
       </c>
@@ -4143,7 +4144,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="333" spans="1:2">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>159</v>
       </c>
@@ -4151,7 +4152,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="334" spans="1:2">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>71</v>
       </c>
@@ -4159,7 +4160,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="335" spans="1:2">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>69</v>
       </c>
@@ -4167,7 +4168,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="336">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>66</v>
       </c>
@@ -4175,7 +4176,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="337">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>80</v>
       </c>
@@ -4183,7 +4184,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="338">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>28</v>
       </c>
@@ -4191,7 +4192,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="339">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>38</v>
       </c>
@@ -4199,7 +4200,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="340">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>42</v>
       </c>
@@ -4207,7 +4208,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="341">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>43</v>
       </c>
@@ -4215,7 +4216,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="342">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>79</v>
       </c>
@@ -4223,7 +4224,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="343">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>88</v>
       </c>
@@ -4231,7 +4232,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="344">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>158</v>
       </c>
@@ -4239,7 +4240,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="345">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>32</v>
       </c>
@@ -4247,7 +4248,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="346">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>31</v>
       </c>
@@ -4255,7 +4256,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="347">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>69</v>
       </c>
@@ -4263,7 +4264,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="348">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>91</v>
       </c>
@@ -4271,7 +4272,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="349">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>89</v>
       </c>
@@ -4279,7 +4280,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="350">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>87</v>
       </c>
@@ -4287,7 +4288,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="351">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>52</v>
       </c>
@@ -4295,7 +4296,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="352">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>90</v>
       </c>
@@ -4303,7 +4304,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="353">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>93</v>
       </c>
@@ -4311,7 +4312,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="354">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>27</v>
       </c>
@@ -4319,7 +4320,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="355">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>46</v>
       </c>
@@ -4327,7 +4328,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="356">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>40</v>
       </c>
@@ -4335,7 +4336,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="357">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>49</v>
       </c>
@@ -4343,7 +4344,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="358">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>83</v>
       </c>
@@ -4351,7 +4352,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="359">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>156</v>
       </c>
@@ -4359,7 +4360,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="360">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>34</v>
       </c>
@@ -4367,7 +4368,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="361">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>36</v>
       </c>
@@ -4375,7 +4376,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="362">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>95</v>
       </c>
@@ -4383,7 +4384,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="363">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>155</v>
       </c>
@@ -4391,7 +4392,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="364">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>26</v>
       </c>
@@ -4399,7 +4400,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="365">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>44</v>
       </c>
@@ -4407,7 +4408,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="366">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>75</v>
       </c>
@@ -4415,7 +4416,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="367">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>97</v>
       </c>
@@ -4423,7 +4424,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="368">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>94</v>
       </c>
@@ -4431,7 +4432,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="369">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>96</v>
       </c>
@@ -4439,7 +4440,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="370">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>152</v>
       </c>
@@ -4447,7 +4448,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="371">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>39</v>
       </c>
@@ -4455,7 +4456,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="372">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>45</v>
       </c>
@@ -4463,7 +4464,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="373">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>81</v>
       </c>
@@ -4471,7 +4472,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="374">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>85</v>
       </c>
@@ -4479,7 +4480,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="375">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>29</v>
       </c>
@@ -4487,7 +4488,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="376">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>35</v>
       </c>
@@ -4495,7 +4496,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="377">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>48</v>
       </c>
@@ -4503,7 +4504,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="378">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>157</v>
       </c>
@@ -4511,7 +4512,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="379">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>30</v>
       </c>
@@ -4519,7 +4520,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="380">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>37</v>
       </c>
@@ -4527,7 +4528,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="381">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>50</v>
       </c>
@@ -4535,7 +4536,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="382">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>154</v>
       </c>
@@ -4543,7 +4544,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="383">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>51</v>
       </c>
@@ -4551,7 +4552,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="384">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>82</v>
       </c>
@@ -4559,7 +4560,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="385">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>159</v>
       </c>
@@ -4567,7 +4568,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="386">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>33</v>
       </c>
@@ -4575,7 +4576,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="387">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>41</v>
       </c>
@@ -4583,7 +4584,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="388">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>71</v>
       </c>
@@ -4591,7 +4592,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="389">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>70</v>
       </c>
@@ -4599,7 +4600,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="390">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>53</v>
       </c>
@@ -4607,7 +4608,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="391">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>47</v>
       </c>
@@ -4615,7 +4616,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="392">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>77</v>
       </c>
@@ -4623,7 +4624,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="393">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>99</v>
       </c>
@@ -4631,7 +4632,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="394">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>83</v>
       </c>
@@ -4639,7 +4640,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="395">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>96</v>
       </c>
@@ -4647,7 +4648,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="396">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>51</v>
       </c>
@@ -4655,7 +4656,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="397">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>45</v>
       </c>
@@ -4663,7 +4664,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="398">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>52</v>
       </c>
@@ -4671,7 +4672,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="399">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>77</v>
       </c>
@@ -4679,7 +4680,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="400">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>48</v>
       </c>
@@ -4687,7 +4688,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="401">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>158</v>
       </c>
@@ -4695,7 +4696,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="402">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>155</v>
       </c>
@@ -4703,7 +4704,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="403">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>32</v>
       </c>
@@ -4711,7 +4712,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="404">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>33</v>
       </c>
@@ -4719,7 +4720,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="405">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>36</v>
       </c>
@@ -4727,7 +4728,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="406">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>42</v>
       </c>
@@ -4735,7 +4736,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="407">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>159</v>
       </c>
@@ -4743,7 +4744,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="408">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>157</v>
       </c>
@@ -4751,7 +4752,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="409">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>44</v>
       </c>
@@ -4759,7 +4760,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="410">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>46</v>
       </c>
@@ -4767,7 +4768,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="411">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>87</v>
       </c>
@@ -4775,7 +4776,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="412">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>97</v>
       </c>
@@ -4783,7 +4784,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="413">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>89</v>
       </c>
@@ -4791,7 +4792,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="414">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>49</v>
       </c>
@@ -4799,7 +4800,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="415">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>66</v>
       </c>
@@ -4807,7 +4808,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="416">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>70</v>
       </c>
@@ -4815,7 +4816,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="417">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>81</v>
       </c>
@@ -4823,7 +4824,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="418">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>35</v>
       </c>
@@ -4831,7 +4832,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="419">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>93</v>
       </c>
@@ -4839,7 +4840,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="420">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>31</v>
       </c>
@@ -4847,7 +4848,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="421">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>38</v>
       </c>
@@ -4855,7 +4856,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="422">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>71</v>
       </c>
@@ -4863,7 +4864,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="423">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>79</v>
       </c>
@@ -4871,7 +4872,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="424">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>29</v>
       </c>
@@ -4879,7 +4880,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="425">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>30</v>
       </c>
@@ -4887,7 +4888,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="426">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>43</v>
       </c>
@@ -4895,7 +4896,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="427">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>99</v>
       </c>
@@ -4903,7 +4904,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="428">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>154</v>
       </c>
@@ -4911,7 +4912,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="429">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>90</v>
       </c>
@@ -4919,7 +4920,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="430">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>91</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="431">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>156</v>
       </c>
@@ -4935,7 +4936,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="432">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>39</v>
       </c>
@@ -4943,7 +4944,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="433">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>40</v>
       </c>
@@ -4951,7 +4952,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="434">
+    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>50</v>
       </c>
@@ -4959,7 +4960,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="435">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>85</v>
       </c>
@@ -4967,7 +4968,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="436">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>26</v>
       </c>
@@ -4975,7 +4976,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="437">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>41</v>
       </c>
@@ -4983,7 +4984,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="438">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>69</v>
       </c>
@@ -4991,7 +4992,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="439">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>82</v>
       </c>
@@ -4999,7 +5000,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="440">
+    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>94</v>
       </c>
@@ -5007,7 +5008,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="441">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>28</v>
       </c>
@@ -5015,7 +5016,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="442">
+    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>27</v>
       </c>
@@ -5023,7 +5024,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="443">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>75</v>
       </c>
@@ -5031,7 +5032,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="444">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>37</v>
       </c>
@@ -5039,7 +5040,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="445">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>47</v>
       </c>
@@ -5047,7 +5048,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="446">
+    <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
         <v>80</v>
       </c>
@@ -5055,7 +5056,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="447">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>88</v>
       </c>
@@ -5063,7 +5064,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="448">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>95</v>
       </c>
@@ -5071,7 +5072,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="449">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>34</v>
       </c>
@@ -5079,7 +5080,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="450">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>53</v>
       </c>
@@ -5087,7 +5088,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="451">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>152</v>
       </c>
@@ -5108,7 +5109,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>